<commit_message>
Add metab reactor design
</commit_message>
<xml_diff>
--- a/exposan/metab_mock/data/CFs.xlsx
+++ b/exposan/metab_mock/data/CFs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\metab_mock\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434221E9-AF1C-426A-B26F-A0674FDDCB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E594718-D65E-4BD5-8D2E-2CACE6D4E65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="585" windowWidth="20745" windowHeight="17865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="89">
   <si>
     <t>-</t>
   </si>
@@ -112,18 +112,24 @@
     <t>polyacrylamide production</t>
   </si>
   <si>
+    <t>oxidation of methanol</t>
+  </si>
+  <si>
     <t>copper sulfate production</t>
   </si>
   <si>
-    <t>oxidation of methanol</t>
-  </si>
-  <si>
-    <t>ethylenediamine production</t>
-  </si>
-  <si>
     <t>sulfuric acid production</t>
   </si>
   <si>
+    <t>dimethylamine production</t>
+  </si>
+  <si>
+    <t>ethylene dichloride production</t>
+  </si>
+  <si>
+    <t>potassium hydroxide production</t>
+  </si>
+  <si>
     <t>activated carbon production, granular from hard coal</t>
   </si>
   <si>
@@ -200,6 +206,12 @@
   </si>
   <si>
     <t>wood chips production, hardwood, at sawmill</t>
+  </si>
+  <si>
+    <t>soda ash, dense, to generic market for neutralising agent</t>
+  </si>
+  <si>
+    <t>calcium carbonate production, precipitated</t>
   </si>
   <si>
     <t>heat pump production, for mini CHP plant</t>
@@ -333,22 +345,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -688,21 +691,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="64.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="12" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.62890625" customWidth="1"/>
+    <col min="2" max="2" width="56.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -720,109 +721,109 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -830,7 +831,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D6">
         <v>2.4085729889497871E-2</v>
@@ -860,7 +861,7 @@
         <v>0.29924253090808589</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -868,7 +869,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D7">
         <v>1.5523619695133691E-2</v>
@@ -898,7 +899,7 @@
         <v>0.2046859087406348</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -906,7 +907,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D8">
         <v>8.3554630099028897E-3</v>
@@ -936,7 +937,7 @@
         <v>6.6262377561846802E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -944,7 +945,7 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D9">
         <v>1.6489182981534571E-3</v>
@@ -974,7 +975,7 @@
         <v>2.2306645702629541E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -982,7 +983,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D10">
         <v>3.0811986745389062</v>
@@ -1012,7 +1013,7 @@
         <v>46.742932603631438</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D11">
         <v>0.57516520443394314</v>
@@ -1050,7 +1051,7 @@
         <v>12.00712352370936</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1058,7 +1059,7 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D12">
         <v>0.58162607988276849</v>
@@ -1088,7 +1089,7 @@
         <v>12.19020931143892</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1096,7 +1097,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D13">
         <v>0.77039105635651262</v>
@@ -1126,7 +1127,7 @@
         <v>15.931775197425949</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -1134,7 +1135,7 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D14">
         <v>6.0073414373162277E-3</v>
@@ -1164,7 +1165,7 @@
         <v>7.9512554236612007E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D15">
         <v>3.5128570270090559E-2</v>
@@ -1202,7 +1203,7 @@
         <v>0.33054909538710009</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D16">
         <v>1.4783903305839801E-2</v>
@@ -1240,7 +1241,7 @@
         <v>0.126040478375435</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -1248,37 +1249,37 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D17">
-        <v>0.19319265301746821</v>
+        <v>3.3897172809095951E-3</v>
       </c>
       <c r="E17">
-        <v>3.7913277856679271</v>
+        <v>0.87011861083147213</v>
       </c>
       <c r="F17">
-        <v>5067.9142035823943</v>
+        <v>13.644208952454941</v>
       </c>
       <c r="G17">
-        <v>0.14425878843980189</v>
+        <v>4.0327925094671381E-3</v>
       </c>
       <c r="H17">
-        <v>2.000739661340539E-6</v>
+        <v>6.0299852025642145E-8</v>
       </c>
       <c r="I17">
-        <v>5.2238003764700042E-5</v>
+        <v>1.853715322424159E-7</v>
       </c>
       <c r="J17">
-        <v>2.311108842998087E-7</v>
+        <v>2.5453935060748422E-7</v>
       </c>
       <c r="K17">
-        <v>2.0220403326919711E-2</v>
+        <v>3.6205549396033511E-4</v>
       </c>
       <c r="L17">
-        <v>0.72499047355210655</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.0336292947182781E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>13</v>
       </c>
@@ -1286,37 +1287,37 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D18">
-        <v>3.3897172809095951E-3</v>
+        <v>0.19319265301746821</v>
       </c>
       <c r="E18">
-        <v>0.87011861083147213</v>
+        <v>3.7913277856679271</v>
       </c>
       <c r="F18">
-        <v>13.644208952454941</v>
+        <v>5067.9142035823943</v>
       </c>
       <c r="G18">
-        <v>4.0327925094671381E-3</v>
+        <v>0.14425878843980189</v>
       </c>
       <c r="H18">
-        <v>6.0299852025642145E-8</v>
+        <v>2.000739661340539E-6</v>
       </c>
       <c r="I18">
-        <v>1.853715322424159E-7</v>
+        <v>5.2238003764700042E-5</v>
       </c>
       <c r="J18">
-        <v>2.5453935060748422E-7</v>
+        <v>2.311108842998087E-7</v>
       </c>
       <c r="K18">
-        <v>3.6205549396033511E-4</v>
+        <v>2.0220403326919711E-2</v>
       </c>
       <c r="L18">
-        <v>5.0336292947182781E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.72499047355210655</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -1324,37 +1325,37 @@
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D19">
-        <v>2.3925494275387021E-2</v>
+        <v>8.2440945087619948E-3</v>
       </c>
       <c r="E19">
-        <v>6.1219761820066756</v>
+        <v>8.1180873696622163E-2</v>
       </c>
       <c r="F19">
-        <v>70.889176881740823</v>
+        <v>6.1078043915780702</v>
       </c>
       <c r="G19">
-        <v>2.9500741918185011E-2</v>
+        <v>4.052641551952609E-4</v>
       </c>
       <c r="H19">
-        <v>3.8161115357277791E-7</v>
+        <v>1.9900118791554861E-8</v>
       </c>
       <c r="I19">
-        <v>1.2244755231587129E-6</v>
+        <v>7.0471539411084789E-8</v>
       </c>
       <c r="J19">
-        <v>9.3704672253178757E-7</v>
+        <v>7.8786002778743982E-9</v>
       </c>
       <c r="K19">
-        <v>4.6371798883808584E-3</v>
+        <v>5.3306619619169875E-4</v>
       </c>
       <c r="L19">
-        <v>0.28402708684996558</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.0788229739628897E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1362,37 +1363,37 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D20">
-        <v>8.2440945087619948E-3</v>
+        <v>7.9323679736229592E-3</v>
       </c>
       <c r="E20">
-        <v>8.1180873696622163E-2</v>
+        <v>2.4738385941837309</v>
       </c>
       <c r="F20">
-        <v>6.1078043915780702</v>
+        <v>23.839381732285322</v>
       </c>
       <c r="G20">
-        <v>4.052641551952609E-4</v>
+        <v>2.0066526614934108E-2</v>
       </c>
       <c r="H20">
-        <v>1.9900118791554861E-8</v>
+        <v>1.1002785083668409E-7</v>
       </c>
       <c r="I20">
-        <v>7.0471539411084789E-8</v>
+        <v>3.3524003279968988E-7</v>
       </c>
       <c r="J20">
-        <v>7.8786002778743982E-9</v>
+        <v>5.2855592935421639E-7</v>
       </c>
       <c r="K20">
-        <v>5.3306619619169875E-4</v>
+        <v>7.3908156206257849E-4</v>
       </c>
       <c r="L20">
-        <v>5.0788229739628897E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.89356054614171E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -1400,37 +1401,37 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D21">
-        <v>5.2143502817840658E-2</v>
+        <v>4.0578937885988051E-3</v>
       </c>
       <c r="E21">
-        <v>8.3093636017746011</v>
+        <v>0.99626041462335335</v>
       </c>
       <c r="F21">
-        <v>37.960671101590172</v>
+        <v>23.932736658197271</v>
       </c>
       <c r="G21">
-        <v>2.6736671732324181E-2</v>
+        <v>3.6421324206076132E-3</v>
       </c>
       <c r="H21">
-        <v>4.1638050250526378E-7</v>
+        <v>1.014253130810726E-7</v>
       </c>
       <c r="I21">
-        <v>1.3938998615257031E-6</v>
+        <v>4.1676460042949509E-7</v>
       </c>
       <c r="J21">
-        <v>1.4034406376134719E-7</v>
+        <v>4.2710039251832932E-7</v>
       </c>
       <c r="K21">
-        <v>7.0857398484638614E-3</v>
+        <v>5.6686092266700614E-4</v>
       </c>
       <c r="L21">
-        <v>0.46916640759150208</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>4.9805082070493327E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>17</v>
       </c>
@@ -1438,37 +1439,37 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D22">
-        <v>1.266994614311171E-2</v>
+        <v>1.3237645096850119E-2</v>
       </c>
       <c r="E22">
-        <v>1.510442676050656</v>
+        <v>2.744984314653903</v>
       </c>
       <c r="F22">
-        <v>84.039229338602951</v>
+        <v>50.724241846065283</v>
       </c>
       <c r="G22">
-        <v>9.3237811391145703E-3</v>
+        <v>8.299040852414204E-3</v>
       </c>
       <c r="H22">
-        <v>2.1999799075220221E-7</v>
+        <v>2.4258105073100372E-7</v>
       </c>
       <c r="I22">
-        <v>1.3780940184872829E-6</v>
+        <v>8.3741838603636462E-7</v>
       </c>
       <c r="J22">
-        <v>3.6433854223773832E-7</v>
+        <v>1.6299951058807961E-7</v>
       </c>
       <c r="K22">
-        <v>2.0927910253944831E-3</v>
+        <v>3.3362119524061049E-3</v>
       </c>
       <c r="L22">
-        <v>9.4568009080592055E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1739175395086841</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>18</v>
       </c>
@@ -1476,37 +1477,37 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D23">
-        <v>8.1715656946625664E-2</v>
+        <v>5.2143502817840658E-2</v>
       </c>
       <c r="E23">
-        <v>16.695362370857929</v>
+        <v>8.3093636017746011</v>
       </c>
       <c r="F23">
-        <v>151.5957962968786</v>
+        <v>37.960671101590172</v>
       </c>
       <c r="G23">
-        <v>4.0575422804887983E-2</v>
+        <v>2.6736671732324181E-2</v>
       </c>
       <c r="H23">
-        <v>9.3018620093473582E-7</v>
+        <v>4.1638050250526378E-7</v>
       </c>
       <c r="I23">
-        <v>3.2334374886886982E-6</v>
+        <v>1.3938998615257031E-6</v>
       </c>
       <c r="J23">
-        <v>1.5319873459483789E-3</v>
+        <v>1.4034406376134719E-7</v>
       </c>
       <c r="K23">
-        <v>1.5473796307994579E-2</v>
+        <v>7.0857398484638614E-3</v>
       </c>
       <c r="L23">
-        <v>1.1548549689732339</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.46916640759150208</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>19</v>
       </c>
@@ -1514,37 +1515,37 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D24">
-        <v>2.4322566518315811E-2</v>
+        <v>1.266994614311171E-2</v>
       </c>
       <c r="E24">
-        <v>7.7850413028470991</v>
+        <v>1.510442676050656</v>
       </c>
       <c r="F24">
-        <v>13.85372954206886</v>
+        <v>84.039229338602951</v>
       </c>
       <c r="G24">
-        <v>2.563212433018366E-3</v>
+        <v>9.3237811391145703E-3</v>
       </c>
       <c r="H24">
-        <v>2.4786864428792091E-7</v>
+        <v>2.1999799075220221E-7</v>
       </c>
       <c r="I24">
-        <v>8.8123114737693013E-7</v>
+        <v>1.3780940184872829E-6</v>
       </c>
       <c r="J24">
-        <v>4.4611866637081026E-9</v>
+        <v>3.6433854223773832E-7</v>
       </c>
       <c r="K24">
-        <v>3.8901585962261868E-3</v>
+        <v>2.0927910253944831E-3</v>
       </c>
       <c r="L24">
-        <v>0.31627244612906141</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>9.4568009080592055E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>20</v>
       </c>
@@ -1552,37 +1553,37 @@
         <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D25">
-        <v>5.6119645022909004E-3</v>
+        <v>8.1715656946625664E-2</v>
       </c>
       <c r="E25">
-        <v>1.8608448721471169</v>
+        <v>16.695362370857929</v>
       </c>
       <c r="F25">
-        <v>15.158814882341369</v>
+        <v>151.5957962968786</v>
       </c>
       <c r="G25">
-        <v>2.0655542316690501E-3</v>
+        <v>4.0575422804887983E-2</v>
       </c>
       <c r="H25">
-        <v>8.637056513253151E-8</v>
+        <v>9.3018620093473582E-7</v>
       </c>
       <c r="I25">
-        <v>1.9403017246688381E-7</v>
+        <v>3.2334374886886982E-6</v>
       </c>
       <c r="J25">
-        <v>2.7684150246652811E-8</v>
+        <v>1.5319873459483789E-3</v>
       </c>
       <c r="K25">
-        <v>5.5145870278407844E-4</v>
+        <v>1.5473796307994579E-2</v>
       </c>
       <c r="L25">
-        <v>8.1045763728104875E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.1548549689732339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>21</v>
       </c>
@@ -1590,37 +1591,37 @@
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D26">
-        <v>2.558611373784361E-2</v>
+        <v>2.4322566518315811E-2</v>
       </c>
       <c r="E26">
-        <v>5.4581544258534311</v>
+        <v>7.7850413028470991</v>
       </c>
       <c r="F26">
-        <v>94.876866999385271</v>
+        <v>13.85372954206886</v>
       </c>
       <c r="G26">
-        <v>2.175820274561405E-2</v>
+        <v>2.563212433018366E-3</v>
       </c>
       <c r="H26">
-        <v>4.6095709976480201E-7</v>
+        <v>2.4786864428792091E-7</v>
       </c>
       <c r="I26">
-        <v>1.558269857075502E-6</v>
+        <v>8.8123114737693013E-7</v>
       </c>
       <c r="J26">
-        <v>7.2012081535820177E-7</v>
+        <v>4.4611866637081026E-9</v>
       </c>
       <c r="K26">
-        <v>5.0274157646736078E-3</v>
+        <v>3.8901585962261868E-3</v>
       </c>
       <c r="L26">
-        <v>0.3884110077629116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.31627244612906141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>22</v>
       </c>
@@ -1628,37 +1629,37 @@
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D27">
-        <v>5.8424163562585344E-3</v>
+        <v>5.6119645022909004E-3</v>
       </c>
       <c r="E27">
-        <v>1.889197380583169</v>
+        <v>1.8608448721471169</v>
       </c>
       <c r="F27">
-        <v>15.738275282157391</v>
+        <v>15.158814882341369</v>
       </c>
       <c r="G27">
-        <v>2.466116899168572E-3</v>
+        <v>2.0655542316690501E-3</v>
       </c>
       <c r="H27">
-        <v>1.126000623516756E-7</v>
+        <v>8.637056513253151E-8</v>
       </c>
       <c r="I27">
-        <v>2.136961262996235E-7</v>
+        <v>1.9403017246688381E-7</v>
       </c>
       <c r="J27">
-        <v>4.486790277554288E-8</v>
+        <v>2.7684150246652811E-8</v>
       </c>
       <c r="K27">
-        <v>5.8080933972364619E-4</v>
+        <v>5.5145870278407844E-4</v>
       </c>
       <c r="L27">
-        <v>8.5443423095504858E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.1045763728104875E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>23</v>
       </c>
@@ -1666,37 +1667,37 @@
         <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D28">
-        <v>1.083467201626463E-4</v>
+        <v>2.558611373784361E-2</v>
       </c>
       <c r="E28">
-        <v>2.8478625916064409E-2</v>
+        <v>5.4581544258534311</v>
       </c>
       <c r="F28">
-        <v>0.23448317519761361</v>
+        <v>94.876866999385271</v>
       </c>
       <c r="G28">
-        <v>5.4890928986476407E-5</v>
+        <v>2.175820274561405E-2</v>
       </c>
       <c r="H28">
-        <v>1.5016679470121821E-9</v>
+        <v>4.6095709976480201E-7</v>
       </c>
       <c r="I28">
-        <v>4.1466197573786109E-9</v>
+        <v>1.558269857075502E-6</v>
       </c>
       <c r="J28">
-        <v>4.7471663537593414E-10</v>
+        <v>7.2012081535820177E-7</v>
       </c>
       <c r="K28">
-        <v>1.8890196040183121E-5</v>
+        <v>5.0274157646736078E-3</v>
       </c>
       <c r="L28">
-        <v>1.541244719329245E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.3884110077629116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>24</v>
       </c>
@@ -1704,37 +1705,37 @@
         <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D29">
-        <v>9.7053818683995909E-3</v>
+        <v>5.8424163562585344E-3</v>
       </c>
       <c r="E29">
-        <v>2.431339071421633</v>
+        <v>1.889197380583169</v>
       </c>
       <c r="F29">
-        <v>40.062615499605947</v>
+        <v>15.738275282157391</v>
       </c>
       <c r="G29">
-        <v>6.0971005043306218E-3</v>
+        <v>2.466116899168572E-3</v>
       </c>
       <c r="H29">
-        <v>1.9166753297345329E-7</v>
+        <v>1.126000623516756E-7</v>
       </c>
       <c r="I29">
-        <v>6.3272577462748359E-7</v>
+        <v>2.136961262996235E-7</v>
       </c>
       <c r="J29">
-        <v>1.147692823803628E-6</v>
+        <v>4.486790277554288E-8</v>
       </c>
       <c r="K29">
-        <v>2.055931900685207E-3</v>
+        <v>5.8080933972364619E-4</v>
       </c>
       <c r="L29">
-        <v>0.12404222539191551</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8.5443423095504858E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>25</v>
       </c>
@@ -1742,37 +1743,37 @@
         <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D30">
-        <v>8.8439159992618702E-3</v>
+        <v>1.083467201626463E-4</v>
       </c>
       <c r="E30">
-        <v>2.3823753515516799</v>
+        <v>2.8478625916064409E-2</v>
       </c>
       <c r="F30">
-        <v>41.107957525360163</v>
+        <v>0.23448317519761361</v>
       </c>
       <c r="G30">
-        <v>6.7225092925464842E-3</v>
+        <v>5.4890928986476407E-5</v>
       </c>
       <c r="H30">
-        <v>1.921305755740457E-7</v>
+        <v>1.5016679470121821E-9</v>
       </c>
       <c r="I30">
-        <v>6.5942261290274099E-7</v>
+        <v>4.1466197573786109E-9</v>
       </c>
       <c r="J30">
-        <v>1.216669575354727E-6</v>
+        <v>4.7471663537593414E-10</v>
       </c>
       <c r="K30">
-        <v>1.075782224101125E-3</v>
+        <v>1.8890196040183121E-5</v>
       </c>
       <c r="L30">
-        <v>0.102909495941138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1.541244719329245E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>26</v>
       </c>
@@ -1780,37 +1781,37 @@
         <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D31">
-        <v>1.8334257094870209E-2</v>
+        <v>9.7053818683995909E-3</v>
       </c>
       <c r="E31">
-        <v>4.7329324315627961</v>
+        <v>2.431339071421633</v>
       </c>
       <c r="F31">
-        <v>72.750752456212268</v>
+        <v>40.062615499605947</v>
       </c>
       <c r="G31">
-        <v>2.1695862334887552E-2</v>
+        <v>6.0971005043306218E-3</v>
       </c>
       <c r="H31">
-        <v>3.2679188577043363E-7</v>
+        <v>1.9166753297345329E-7</v>
       </c>
       <c r="I31">
-        <v>1.0589492607565189E-6</v>
+        <v>6.3272577462748359E-7</v>
       </c>
       <c r="J31">
-        <v>7.4315239446369308E-7</v>
+        <v>1.147692823803628E-6</v>
       </c>
       <c r="K31">
-        <v>3.6123374860579801E-3</v>
+        <v>2.055931900685207E-3</v>
       </c>
       <c r="L31">
-        <v>0.25703833481078792</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.12404222539191551</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>27</v>
       </c>
@@ -1818,37 +1819,37 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D32">
-        <v>3.0570032379960019E-2</v>
+        <v>8.8439159992618702E-3</v>
       </c>
       <c r="E32">
-        <v>7.5374231306390671</v>
+        <v>2.3823753515516799</v>
       </c>
       <c r="F32">
-        <v>96.108304693822504</v>
+        <v>41.107957525360163</v>
       </c>
       <c r="G32">
-        <v>2.6274536544906021E-2</v>
+        <v>6.7225092925464842E-3</v>
       </c>
       <c r="H32">
-        <v>4.839049346533876E-7</v>
+        <v>1.921305755740457E-7</v>
       </c>
       <c r="I32">
-        <v>1.5985549319753899E-6</v>
+        <v>6.5942261290274099E-7</v>
       </c>
       <c r="J32">
-        <v>1.102939829597071E-6</v>
+        <v>1.216669575354727E-6</v>
       </c>
       <c r="K32">
-        <v>6.4903939922454357E-3</v>
+        <v>1.075782224101125E-3</v>
       </c>
       <c r="L32">
-        <v>0.46080365641305038</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.102909495941138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1">
         <v>28</v>
       </c>
@@ -1856,37 +1857,37 @@
         <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D33">
-        <v>1.837773173045688E-2</v>
+        <v>1.8334257094870209E-2</v>
       </c>
       <c r="E33">
-        <v>4.0364792052818812</v>
+        <v>4.7329324315627961</v>
       </c>
       <c r="F33">
-        <v>49.085369762022673</v>
+        <v>72.750752456212268</v>
       </c>
       <c r="G33">
-        <v>1.0770280576346609E-2</v>
+        <v>2.1695862334887552E-2</v>
       </c>
       <c r="H33">
-        <v>2.345644405686527E-7</v>
+        <v>3.2679188577043363E-7</v>
       </c>
       <c r="I33">
-        <v>1.2867664815977479E-6</v>
+        <v>1.0589492607565189E-6</v>
       </c>
       <c r="J33">
-        <v>3.7988190422336329E-7</v>
+        <v>7.4315239446369308E-7</v>
       </c>
       <c r="K33">
-        <v>2.862396526969551E-3</v>
+        <v>3.6123374860579801E-3</v>
       </c>
       <c r="L33">
-        <v>0.26141646303301358</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.25703833481078792</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1">
         <v>29</v>
       </c>
@@ -1894,37 +1895,37 @@
         <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D34">
-        <v>1.3142923154722579E-2</v>
+        <v>3.0570032379960019E-2</v>
       </c>
       <c r="E34">
-        <v>2.80544634987444</v>
+        <v>7.5374231306390671</v>
       </c>
       <c r="F34">
-        <v>40.572079413438388</v>
+        <v>96.108304693822504</v>
       </c>
       <c r="G34">
-        <v>7.1859575439039963E-3</v>
+        <v>2.6274536544906021E-2</v>
       </c>
       <c r="H34">
-        <v>2.1203717220722589E-7</v>
+        <v>4.839049346533876E-7</v>
       </c>
       <c r="I34">
-        <v>8.0192505852314772E-7</v>
+        <v>1.5985549319753899E-6</v>
       </c>
       <c r="J34">
-        <v>6.7813608167965557E-7</v>
+        <v>1.102939829597071E-6</v>
       </c>
       <c r="K34">
-        <v>2.752549812912682E-3</v>
+        <v>6.4903939922454357E-3</v>
       </c>
       <c r="L34">
-        <v>0.17076156472354739</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.46080365641305038</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1">
         <v>30</v>
       </c>
@@ -1932,37 +1933,37 @@
         <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D35">
-        <v>7.8971147091447518E-4</v>
+        <v>1.837773173045688E-2</v>
       </c>
       <c r="E35">
-        <v>1.497583267103773</v>
+        <v>4.0364792052818812</v>
       </c>
       <c r="F35">
-        <v>3.991114980327958</v>
+        <v>49.085369762022673</v>
       </c>
       <c r="G35">
-        <v>3.328639574364561E-4</v>
+        <v>1.0770280576346609E-2</v>
       </c>
       <c r="H35">
-        <v>1.063672413906079E-8</v>
+        <v>2.345644405686527E-7</v>
       </c>
       <c r="I35">
-        <v>6.7022443812690574E-8</v>
+        <v>1.2867664815977479E-6</v>
       </c>
       <c r="J35">
-        <v>4.4377564108912738E-5</v>
+        <v>3.7988190422336329E-7</v>
       </c>
       <c r="K35">
-        <v>1.1117054057199091E-4</v>
+        <v>2.862396526969551E-3</v>
       </c>
       <c r="L35">
-        <v>5.3747762890801482E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.26141646303301358</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1">
         <v>31</v>
       </c>
@@ -1970,37 +1971,37 @@
         <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D36">
-        <v>6.9760670440629752E-2</v>
+        <v>1.3142923154722579E-2</v>
       </c>
       <c r="E36">
-        <v>16.435932633480331</v>
+        <v>2.80544634987444</v>
       </c>
       <c r="F36">
-        <v>230.00896067579939</v>
+        <v>40.572079413438388</v>
       </c>
       <c r="G36">
-        <v>5.2195174187899623E-2</v>
+        <v>7.1859575439039963E-3</v>
       </c>
       <c r="H36">
-        <v>9.3228819424309317E-7</v>
+        <v>2.1203717220722589E-7</v>
       </c>
       <c r="I36">
-        <v>4.3051743304767073E-6</v>
+        <v>8.0192505852314772E-7</v>
       </c>
       <c r="J36">
-        <v>1.128703274363726E-6</v>
+        <v>6.7813608167965557E-7</v>
       </c>
       <c r="K36">
-        <v>1.586607216996231E-2</v>
+        <v>2.752549812912682E-3</v>
       </c>
       <c r="L36">
-        <v>0.93542558645704776</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.17076156472354739</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1">
         <v>32</v>
       </c>
@@ -2008,37 +2009,37 @@
         <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D37">
-        <v>1.729369817341835E-3</v>
+        <v>7.8971147091447518E-4</v>
       </c>
       <c r="E37">
-        <v>0.53365016395323761</v>
+        <v>1.497583267103773</v>
       </c>
       <c r="F37">
-        <v>4.757248862071684</v>
+        <v>3.991114980327958</v>
       </c>
       <c r="G37">
-        <v>7.1008347110269529E-4</v>
+        <v>3.328639574364561E-4</v>
       </c>
       <c r="H37">
-        <v>2.9347377458012161E-8</v>
+        <v>1.063672413906079E-8</v>
       </c>
       <c r="I37">
-        <v>5.2851030390616487E-8</v>
+        <v>6.7022443812690574E-8</v>
       </c>
       <c r="J37">
-        <v>1.8579593526604281E-7</v>
+        <v>4.4377564108912738E-5</v>
       </c>
       <c r="K37">
-        <v>1.928125833579233E-4</v>
+        <v>1.1117054057199091E-4</v>
       </c>
       <c r="L37">
-        <v>2.2266509013954178E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.3747762890801482E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1">
         <v>33</v>
       </c>
@@ -2046,37 +2047,37 @@
         <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D38">
-        <v>5.8680602720372207E-4</v>
+        <v>6.9760670440629752E-2</v>
       </c>
       <c r="E38">
-        <v>0.12666928515636719</v>
+        <v>16.435932633480331</v>
       </c>
       <c r="F38">
-        <v>1.7567298611708679</v>
+        <v>230.00896067579939</v>
       </c>
       <c r="G38">
-        <v>2.9222833144640072E-4</v>
+        <v>5.2195174187899623E-2</v>
       </c>
       <c r="H38">
-        <v>2.0666535932371688E-8</v>
+        <v>9.3228819424309317E-7</v>
       </c>
       <c r="I38">
-        <v>2.3443697641855949E-8</v>
+        <v>4.3051743304767073E-6</v>
       </c>
       <c r="J38">
-        <v>1.8086093102872211E-8</v>
+        <v>1.128703274363726E-6</v>
       </c>
       <c r="K38">
-        <v>8.5712235957590674E-5</v>
+        <v>1.586607216996231E-2</v>
       </c>
       <c r="L38">
-        <v>6.1015907366098014E-3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.93542558645704776</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1">
         <v>34</v>
       </c>
@@ -2084,37 +2085,37 @@
         <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D39">
-        <v>8.083326645578838</v>
+        <v>1.729369817341835E-3</v>
       </c>
       <c r="E39">
-        <v>1838.642112699057</v>
+        <v>0.53365016395323761</v>
       </c>
       <c r="F39">
-        <v>41884.928290196724</v>
+        <v>4.757248862071684</v>
       </c>
       <c r="G39">
-        <v>5.628505070280263</v>
+        <v>7.1008347110269529E-4</v>
       </c>
       <c r="H39">
-        <v>9.7193983960504446E-4</v>
+        <v>2.9347377458012161E-8</v>
       </c>
       <c r="I39">
-        <v>5.8323689390971437E-4</v>
+        <v>5.2851030390616487E-8</v>
       </c>
       <c r="J39">
-        <v>1.5740203519961561E-4</v>
+        <v>1.8579593526604281E-7</v>
       </c>
       <c r="K39">
-        <v>2.0552221910994501</v>
+        <v>1.928125833579233E-4</v>
       </c>
       <c r="L39">
-        <v>128.10324107041629</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.2266509013954178E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1">
         <v>35</v>
       </c>
@@ -2122,37 +2123,37 @@
         <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D40">
-        <v>2.4834726156618161E-2</v>
+        <v>5.8680602720372207E-4</v>
       </c>
       <c r="E40">
-        <v>5.7714418558232783</v>
+        <v>0.12666928515636719</v>
       </c>
       <c r="F40">
-        <v>73.445618295573496</v>
+        <v>1.7567298611708679</v>
       </c>
       <c r="G40">
-        <v>1.7387778736338899E-2</v>
+        <v>2.9222833144640072E-4</v>
       </c>
       <c r="H40">
-        <v>5.5485058431763002E-7</v>
+        <v>2.0666535932371688E-8</v>
       </c>
       <c r="I40">
-        <v>1.4009221001058801E-6</v>
+        <v>2.3443697641855949E-8</v>
       </c>
       <c r="J40">
-        <v>1.442540878762118E-5</v>
+        <v>1.8086093102872211E-8</v>
       </c>
       <c r="K40">
-        <v>5.3729499992496103E-3</v>
+        <v>8.5712235957590674E-5</v>
       </c>
       <c r="L40">
-        <v>0.34757670108633071</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>6.1015907366098014E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1">
         <v>36</v>
       </c>
@@ -2160,37 +2161,37 @@
         <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D41">
-        <v>1.566139108987959E-2</v>
+        <v>8.083326645578838</v>
       </c>
       <c r="E41">
-        <v>2.6479601501207548</v>
+        <v>1838.642112699057</v>
       </c>
       <c r="F41">
-        <v>61.146755636986597</v>
+        <v>41884.928290196724</v>
       </c>
       <c r="G41">
-        <v>1.073785332224979E-2</v>
+        <v>5.628505070280263</v>
       </c>
       <c r="H41">
-        <v>2.1889577708851271E-7</v>
+        <v>9.7193983960504446E-4</v>
       </c>
       <c r="I41">
-        <v>1.0320849524209799E-6</v>
+        <v>5.8323689390971437E-4</v>
       </c>
       <c r="J41">
-        <v>2.2953511000388489E-7</v>
+        <v>1.5740203519961561E-4</v>
       </c>
       <c r="K41">
-        <v>2.6667321271850951E-3</v>
+        <v>2.0552221910994501</v>
       </c>
       <c r="L41">
-        <v>0.16779416204456049</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>128.10324107041629</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1">
         <v>37</v>
       </c>
@@ -2198,37 +2199,37 @@
         <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D42">
-        <v>2.529411095024988E-2</v>
+        <v>2.4834726156618161E-2</v>
       </c>
       <c r="E42">
-        <v>5.5587649312100664</v>
+        <v>5.7714418558232783</v>
       </c>
       <c r="F42">
-        <v>238.51603904599591</v>
+        <v>73.445618295573496</v>
       </c>
       <c r="G42">
-        <v>1.7487302221629201E-2</v>
+        <v>1.7387778736338899E-2</v>
       </c>
       <c r="H42">
-        <v>1.1734112409297401E-5</v>
+        <v>5.5485058431763002E-7</v>
       </c>
       <c r="I42">
-        <v>3.0193453571297851E-6</v>
+        <v>1.4009221001058801E-6</v>
       </c>
       <c r="J42">
-        <v>2.6698710974950831E-7</v>
+        <v>1.442540878762118E-5</v>
       </c>
       <c r="K42">
-        <v>1.5390240000981621E-2</v>
+        <v>5.3729499992496103E-3</v>
       </c>
       <c r="L42">
-        <v>0.31847640700611313</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.34757670108633071</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1">
         <v>38</v>
       </c>
@@ -2236,37 +2237,37 @@
         <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D43">
-        <v>12.073656963151519</v>
+        <v>1.566139108987959E-2</v>
       </c>
       <c r="E43">
-        <v>793.73422934988741</v>
+        <v>2.6479601501207548</v>
       </c>
       <c r="F43">
-        <v>280525.18743038143</v>
+        <v>61.146755636986597</v>
       </c>
       <c r="G43">
-        <v>9.4116718016510532</v>
+        <v>1.073785332224979E-2</v>
       </c>
       <c r="H43">
-        <v>7.5720393093265856E-4</v>
+        <v>2.1889577708851271E-7</v>
       </c>
       <c r="I43">
-        <v>2.950386281220684E-3</v>
+        <v>1.0320849524209799E-6</v>
       </c>
       <c r="J43">
-        <v>4.3254825256180202E-5</v>
+        <v>2.2953511000388489E-7</v>
       </c>
       <c r="K43">
-        <v>1.8179095397138281</v>
+        <v>2.6667321271850951E-3</v>
       </c>
       <c r="L43">
-        <v>73.150321394177197</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.16779416204456049</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1">
         <v>39</v>
       </c>
@@ -2274,37 +2275,37 @@
         <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D44">
-        <v>3.1754974359125761E-4</v>
+        <v>2.529411095024988E-2</v>
       </c>
       <c r="E44">
-        <v>4.3620545619324887E-2</v>
+        <v>5.5587649312100664</v>
       </c>
       <c r="F44">
-        <v>0.31566699560240857</v>
+        <v>238.51603904599591</v>
       </c>
       <c r="G44">
-        <v>1.2583657005000161E-4</v>
+        <v>1.7487302221629201E-2</v>
       </c>
       <c r="H44">
-        <v>3.207018796531503E-9</v>
+        <v>1.1734112409297401E-5</v>
       </c>
       <c r="I44">
-        <v>8.3999242657780522E-9</v>
+        <v>3.0193453571297851E-6</v>
       </c>
       <c r="J44">
-        <v>1.865020805512048E-9</v>
+        <v>2.6698710974950831E-7</v>
       </c>
       <c r="K44">
-        <v>5.0141379990399041E-4</v>
+        <v>1.5390240000981621E-2</v>
       </c>
       <c r="L44">
-        <v>5.5270447981638554E-3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.31847640700611313</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1">
         <v>40</v>
       </c>
@@ -2312,37 +2313,37 @@
         <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="D45">
-        <v>1.003448479427718E-4</v>
+        <v>12.073656963151519</v>
       </c>
       <c r="E45">
-        <v>2.4105560931567759E-2</v>
+        <v>793.73422934988741</v>
       </c>
       <c r="F45">
-        <v>0.24121976265892339</v>
+        <v>280525.18743038143</v>
       </c>
       <c r="G45">
-        <v>1.2961401740341349E-4</v>
+        <v>9.4116718016510532</v>
       </c>
       <c r="H45">
-        <v>2.9856582093386632E-9</v>
+        <v>7.5720393093265856E-4</v>
       </c>
       <c r="I45">
-        <v>5.0469385244302284E-9</v>
+        <v>2.950386281220684E-3</v>
       </c>
       <c r="J45">
-        <v>3.0811543996603108E-9</v>
+        <v>4.3254825256180202E-5</v>
       </c>
       <c r="K45">
-        <v>1.420256057079002E-5</v>
+        <v>1.8179095397138281</v>
       </c>
       <c r="L45">
-        <v>2.3539215776325309E-3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>73.150321394177197</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1">
         <v>41</v>
       </c>
@@ -2350,37 +2351,37 @@
         <v>59</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D46">
-        <v>1.3586363718418691E-4</v>
+        <v>3.1754974359125761E-4</v>
       </c>
       <c r="E46">
-        <v>2.879392197377053E-2</v>
+        <v>4.3620545619324887E-2</v>
       </c>
       <c r="F46">
-        <v>0.22485623704282001</v>
+        <v>0.31566699560240857</v>
       </c>
       <c r="G46">
-        <v>9.7273639058382955E-5</v>
+        <v>1.2583657005000161E-4</v>
       </c>
       <c r="H46">
-        <v>3.2699375172001021E-9</v>
+        <v>3.207018796531503E-9</v>
       </c>
       <c r="I46">
-        <v>4.9598226163940397E-9</v>
+        <v>8.3999242657780522E-9</v>
       </c>
       <c r="J46">
-        <v>2.3202315639227799E-9</v>
+        <v>1.865020805512048E-9</v>
       </c>
       <c r="K46">
-        <v>3.6893188619067367E-5</v>
+        <v>5.0141379990399041E-4</v>
       </c>
       <c r="L46">
-        <v>2.7123630613338501E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.5270447981638554E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1">
         <v>42</v>
       </c>
@@ -2388,37 +2389,37 @@
         <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D47">
-        <v>10.96675446147227</v>
+        <v>1.003448479427718E-4</v>
       </c>
       <c r="E47">
-        <v>222.03739105475341</v>
+        <v>2.4105560931567759E-2</v>
       </c>
       <c r="F47">
-        <v>288133.39530135121</v>
+        <v>0.24121976265892339</v>
       </c>
       <c r="G47">
-        <v>8.3307858410089075</v>
+        <v>1.2961401740341349E-4</v>
       </c>
       <c r="H47">
-        <v>1.9573542077655999E-4</v>
+        <v>2.9856582093386632E-9</v>
       </c>
       <c r="I47">
-        <v>3.0168355765251222E-3</v>
+        <v>5.0469385244302284E-9</v>
       </c>
       <c r="J47">
-        <v>1.285933162367626E-5</v>
+        <v>3.0811543996603108E-9</v>
       </c>
       <c r="K47">
-        <v>1.1906933143031191</v>
+        <v>1.420256057079002E-5</v>
       </c>
       <c r="L47">
-        <v>42.417712495063107</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.3539215776325309E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1">
         <v>43</v>
       </c>
@@ -2426,37 +2427,37 @@
         <v>61</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D48">
-        <v>17.715975293179049</v>
+        <v>1.3586363718418691E-4</v>
       </c>
       <c r="E48">
-        <v>1996.4730784102189</v>
+        <v>2.879392197377053E-2</v>
       </c>
       <c r="F48">
-        <v>80529.541872176182</v>
+        <v>0.22485623704282001</v>
       </c>
       <c r="G48">
-        <v>5.8868776447763764</v>
+        <v>9.7273639058382955E-5</v>
       </c>
       <c r="H48">
-        <v>8.9598754434556905E-4</v>
+        <v>3.2699375172001021E-9</v>
       </c>
       <c r="I48">
-        <v>1.1361135190685141E-3</v>
+        <v>4.9598226163940397E-9</v>
       </c>
       <c r="J48">
-        <v>2.1114453405733191E-4</v>
+        <v>2.3202315639227799E-9</v>
       </c>
       <c r="K48">
-        <v>2.392430623871705</v>
+        <v>3.6893188619067367E-5</v>
       </c>
       <c r="L48">
-        <v>154.56538276201681</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.7123630613338501E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1">
         <v>44</v>
       </c>
@@ -2464,37 +2465,37 @@
         <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D49">
-        <v>41.798208916250637</v>
+        <v>6.8910040030967512E-3</v>
       </c>
       <c r="E49">
-        <v>6538.3445226792292</v>
+        <v>1.6532762811102719</v>
       </c>
       <c r="F49">
-        <v>473227.82343392831</v>
+        <v>31.22873764683921</v>
       </c>
       <c r="G49">
-        <v>28.527884792017499</v>
+        <v>8.0388308997974764E-3</v>
       </c>
       <c r="H49">
-        <v>2.5388327956498971E-3</v>
+        <v>1.377273739732079E-7</v>
       </c>
       <c r="I49">
-        <v>5.4850751871178723E-3</v>
+        <v>4.6651458217602198E-7</v>
       </c>
       <c r="J49">
-        <v>4.3768357340257891E-4</v>
+        <v>9.4135315104092812E-8</v>
       </c>
       <c r="K49">
-        <v>8.2178165397930432</v>
+        <v>1.264085648386495E-3</v>
       </c>
       <c r="L49">
-        <v>442.44541478883809</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.1038172920574095</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1">
         <v>45</v>
       </c>
@@ -2502,37 +2503,37 @@
         <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D50">
-        <v>7.460321860185827</v>
+        <v>1.7978724938024109E-3</v>
       </c>
       <c r="E50">
-        <v>862.96354071645169</v>
+        <v>0.33787630406826968</v>
       </c>
       <c r="F50">
-        <v>65049.847672636082</v>
+        <v>11.135209167145719</v>
       </c>
       <c r="G50">
-        <v>3.8834166227687841</v>
+        <v>3.013602884809606E-3</v>
       </c>
       <c r="H50">
-        <v>2.026175521760005E-4</v>
+        <v>3.9777239518568102E-8</v>
       </c>
       <c r="I50">
-        <v>9.0054570177005482E-4</v>
+        <v>1.361537393125253E-7</v>
       </c>
       <c r="J50">
-        <v>5.9520121118880387E-5</v>
+        <v>2.8430519595415051E-8</v>
       </c>
       <c r="K50">
-        <v>1.0734649004664589</v>
+        <v>2.9389134309588911E-4</v>
       </c>
       <c r="L50">
-        <v>65.772156640798912</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2.356305240440959E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1">
         <v>46</v>
       </c>
@@ -2540,37 +2541,37 @@
         <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D51">
-        <v>4.3408052644170887</v>
+        <v>10.96675446147227</v>
       </c>
       <c r="E51">
-        <v>508.28407955317613</v>
+        <v>222.03739105475341</v>
       </c>
       <c r="F51">
-        <v>86910.506871515929</v>
+        <v>288133.39530135121</v>
       </c>
       <c r="G51">
-        <v>3.45761597293273</v>
+        <v>8.3307858410089075</v>
       </c>
       <c r="H51">
-        <v>5.9768738666675641E-4</v>
+        <v>1.9573542077655999E-4</v>
       </c>
       <c r="I51">
-        <v>8.7987270135620236E-4</v>
+        <v>3.0168355765251222E-3</v>
       </c>
       <c r="J51">
-        <v>2.860709891426959E-5</v>
+        <v>1.285933162367626E-5</v>
       </c>
       <c r="K51">
-        <v>0.89494473894098947</v>
+        <v>1.1906933143031191</v>
       </c>
       <c r="L51">
-        <v>36.303510780944848</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>42.417712495063107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1">
         <v>47</v>
       </c>
@@ -2578,37 +2579,37 @@
         <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D52">
-        <v>17.938025614823498</v>
+        <v>17.715975293179049</v>
       </c>
       <c r="E52">
-        <v>1283.1037262435941</v>
+        <v>1996.4730784102189</v>
       </c>
       <c r="F52">
-        <v>1573301.7234750569</v>
+        <v>80529.541872176182</v>
       </c>
       <c r="G52">
-        <v>13.28577068400573</v>
+        <v>5.8868776447763764</v>
       </c>
       <c r="H52">
-        <v>2.4889589639819419E-3</v>
+        <v>8.9598754434556905E-4</v>
       </c>
       <c r="I52">
-        <v>4.4861706195940066E-3</v>
+        <v>1.1361135190685141E-3</v>
       </c>
       <c r="J52">
-        <v>7.5177137059215758E-5</v>
+        <v>2.1114453405733191E-4</v>
       </c>
       <c r="K52">
-        <v>3.7990966488767199</v>
+        <v>2.392430623871705</v>
       </c>
       <c r="L52">
-        <v>111.08209324813841</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>154.56538276201681</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1">
         <v>48</v>
       </c>
@@ -2616,37 +2617,37 @@
         <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D53">
-        <v>0.14212227461096291</v>
+        <v>41.798208916250637</v>
       </c>
       <c r="E53">
-        <v>9.2510249269176565</v>
+        <v>6538.3445226792292</v>
       </c>
       <c r="F53">
-        <v>3189.5736873935762</v>
+        <v>473227.82343392831</v>
       </c>
       <c r="G53">
-        <v>0.10531292230566761</v>
+        <v>28.527884792017499</v>
       </c>
       <c r="H53">
-        <v>2.012121634216439E-5</v>
+        <v>2.5388327956498971E-3</v>
       </c>
       <c r="I53">
-        <v>3.5992972430286133E-5</v>
+        <v>5.4850751871178723E-3</v>
       </c>
       <c r="J53">
-        <v>5.2616424627118548E-7</v>
+        <v>4.3768357340257891E-4</v>
       </c>
       <c r="K53">
-        <v>2.9716488363209219E-2</v>
+        <v>8.2178165397930432</v>
       </c>
       <c r="L53">
-        <v>0.85457572715826635</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>442.44541478883809</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1">
         <v>49</v>
       </c>
@@ -2654,37 +2655,37 @@
         <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D54">
-        <v>4.2427303129558887E-3</v>
+        <v>7.460321860185827</v>
       </c>
       <c r="E54">
-        <v>1.045907075826479</v>
+        <v>862.96354071645169</v>
       </c>
       <c r="F54">
-        <v>20.68704960381945</v>
+        <v>65049.847672636082</v>
       </c>
       <c r="G54">
-        <v>2.6258440202684159E-3</v>
+        <v>3.8834166227687841</v>
       </c>
       <c r="H54">
-        <v>7.9378697614191662E-8</v>
+        <v>2.026175521760005E-4</v>
       </c>
       <c r="I54">
-        <v>2.6982505875321181E-7</v>
+        <v>9.0054570177005482E-4</v>
       </c>
       <c r="J54">
-        <v>3.8003004810527681E-8</v>
+        <v>5.9520121118880387E-5</v>
       </c>
       <c r="K54">
-        <v>5.4855084316208624E-4</v>
+        <v>1.0734649004664589</v>
       </c>
       <c r="L54">
-        <v>5.4606298275374193E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>65.772156640798912</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1">
         <v>50</v>
       </c>
@@ -2692,37 +2693,37 @@
         <v>68</v>
       </c>
       <c r="C55" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D55">
-        <v>4.2534751237281843E-2</v>
+        <v>4.3408052644170887</v>
       </c>
       <c r="E55">
-        <v>10.036834952923479</v>
+        <v>508.28407955317613</v>
       </c>
       <c r="F55">
-        <v>185.17769364746439</v>
+        <v>86910.506871515929</v>
       </c>
       <c r="G55">
-        <v>2.8555427451633E-2</v>
+        <v>3.45761597293273</v>
       </c>
       <c r="H55">
-        <v>7.3206176091797782E-7</v>
+        <v>5.9768738666675641E-4</v>
       </c>
       <c r="I55">
-        <v>2.567299609836942E-6</v>
+        <v>8.7987270135620236E-4</v>
       </c>
       <c r="J55">
-        <v>3.2246869814908462E-7</v>
+        <v>2.860709891426959E-5</v>
       </c>
       <c r="K55">
-        <v>6.8671320664443602E-3</v>
+        <v>0.89494473894098947</v>
       </c>
       <c r="L55">
-        <v>0.54896370334877764</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>36.303510780944848</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1">
         <v>51</v>
       </c>
@@ -2730,37 +2731,37 @@
         <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D56">
-        <v>2.000310745204657E-3</v>
+        <v>17.938025614823498</v>
       </c>
       <c r="E56">
-        <v>0.58207696828590905</v>
+        <v>1283.1037262435941</v>
       </c>
       <c r="F56">
-        <v>6.5147445229833831</v>
+        <v>1573301.7234750569</v>
       </c>
       <c r="G56">
-        <v>6.1035685990956986E-3</v>
+        <v>13.28577068400573</v>
       </c>
       <c r="H56">
-        <v>6.3544295964226045E-8</v>
+        <v>2.4889589639819419E-3</v>
       </c>
       <c r="I56">
-        <v>2.1652695165120729E-7</v>
+        <v>4.4861706195940066E-3</v>
       </c>
       <c r="J56">
-        <v>1.8550017361081969E-8</v>
+        <v>7.5177137059215758E-5</v>
       </c>
       <c r="K56">
-        <v>2.5472145819678878E-3</v>
+        <v>3.7990966488767199</v>
       </c>
       <c r="L56">
-        <v>1.8724443118126741E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>111.08209324813841</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1">
         <v>52</v>
       </c>
@@ -2768,33 +2769,185 @@
         <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D57">
+        <v>0.14212227461096291</v>
+      </c>
+      <c r="E57">
+        <v>9.2510249269176565</v>
+      </c>
+      <c r="F57">
+        <v>3189.5736873935762</v>
+      </c>
+      <c r="G57">
+        <v>0.10531292230566761</v>
+      </c>
+      <c r="H57">
+        <v>2.012121634216439E-5</v>
+      </c>
+      <c r="I57">
+        <v>3.5992972430286133E-5</v>
+      </c>
+      <c r="J57">
+        <v>5.2616424627118548E-7</v>
+      </c>
+      <c r="K57">
+        <v>2.9716488363209219E-2</v>
+      </c>
+      <c r="L57">
+        <v>0.85457572715826635</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="1">
+        <v>53</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58">
+        <v>4.2427303129558887E-3</v>
+      </c>
+      <c r="E58">
+        <v>1.045907075826479</v>
+      </c>
+      <c r="F58">
+        <v>20.68704960381945</v>
+      </c>
+      <c r="G58">
+        <v>2.6258440202684159E-3</v>
+      </c>
+      <c r="H58">
+        <v>7.9378697614191662E-8</v>
+      </c>
+      <c r="I58">
+        <v>2.6982505875321181E-7</v>
+      </c>
+      <c r="J58">
+        <v>3.8003004810527681E-8</v>
+      </c>
+      <c r="K58">
+        <v>5.4855084316208624E-4</v>
+      </c>
+      <c r="L58">
+        <v>5.4606298275374193E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="1">
+        <v>54</v>
+      </c>
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59">
+        <v>4.2534751237281843E-2</v>
+      </c>
+      <c r="E59">
+        <v>10.036834952923479</v>
+      </c>
+      <c r="F59">
+        <v>185.17769364746439</v>
+      </c>
+      <c r="G59">
+        <v>2.8555427451633E-2</v>
+      </c>
+      <c r="H59">
+        <v>7.3206176091797782E-7</v>
+      </c>
+      <c r="I59">
+        <v>2.567299609836942E-6</v>
+      </c>
+      <c r="J59">
+        <v>3.2246869814908462E-7</v>
+      </c>
+      <c r="K59">
+        <v>6.8671320664443602E-3</v>
+      </c>
+      <c r="L59">
+        <v>0.54896370334877764</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="1">
+        <v>55</v>
+      </c>
+      <c r="B60" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60">
+        <v>2.000310745204657E-3</v>
+      </c>
+      <c r="E60">
+        <v>0.58207696828590905</v>
+      </c>
+      <c r="F60">
+        <v>6.5147445229833831</v>
+      </c>
+      <c r="G60">
+        <v>6.1035685990956986E-3</v>
+      </c>
+      <c r="H60">
+        <v>6.3544295964226045E-8</v>
+      </c>
+      <c r="I60">
+        <v>2.1652695165120729E-7</v>
+      </c>
+      <c r="J60">
+        <v>1.8550017361081969E-8</v>
+      </c>
+      <c r="K60">
+        <v>2.5472145819678878E-3</v>
+      </c>
+      <c r="L60">
+        <v>1.8724443118126741E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="1">
+        <v>56</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61">
         <v>7.3793076438428723E-5</v>
       </c>
-      <c r="E57">
+      <c r="E61">
         <v>7.4211120334528327E-2</v>
       </c>
-      <c r="F57">
+      <c r="F61">
         <v>0.1629409232385339</v>
       </c>
-      <c r="G57">
+      <c r="G61">
         <v>1.9485050688014222E-5</v>
       </c>
-      <c r="H57">
+      <c r="H61">
         <v>1.2123422985395279E-9</v>
       </c>
-      <c r="I57">
+      <c r="I61">
         <v>2.3010230741065661E-9</v>
       </c>
-      <c r="J57">
+      <c r="J61">
         <v>8.5888518112481996E-9</v>
       </c>
-      <c r="K57">
+      <c r="K61">
         <v>6.0465437087421874E-6</v>
       </c>
-      <c r="L57">
+      <c r="L61">
         <v>1.074330522005385E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add impact items CFs
</commit_message>
<xml_diff>
--- a/exposan/metab_mock/data/CFs.xlsx
+++ b/exposan/metab_mock/data/CFs.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\metab_mock\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E594718-D65E-4BD5-8D2E-2CACE6D4E65A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA39D12C-5CC0-4D36-95E2-5F6D274481D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24405" yWindow="105" windowWidth="17280" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="exported" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="153">
   <si>
     <t>-</t>
   </si>
@@ -79,28 +92,40 @@
     <t>maximum incremental reactivity (MIR)</t>
   </si>
   <si>
-    <t>steel production, electric, chromium steel 18/8</t>
-  </si>
-  <si>
-    <t>polystyrene foam slab for perimeter insulation</t>
-  </si>
-  <si>
-    <t>stone wool production, packed</t>
-  </si>
-  <si>
-    <t>cellulose fibre production</t>
-  </si>
-  <si>
-    <t>concrete slab production</t>
-  </si>
-  <si>
-    <t>concrete production 20MPa</t>
-  </si>
-  <si>
-    <t>concrete production 25MPa</t>
-  </si>
-  <si>
-    <t>concrete production 35MPa</t>
+    <t>market for steel, chromium steel 18/8</t>
+  </si>
+  <si>
+    <t>market for steel, chromium steel 18/8, hot rolled</t>
+  </si>
+  <si>
+    <t>market for stone wool</t>
+  </si>
+  <si>
+    <t>market for stone wool, packed</t>
+  </si>
+  <si>
+    <t>market for concrete slab</t>
+  </si>
+  <si>
+    <t>market for concrete, normal</t>
+  </si>
+  <si>
+    <t>market for concrete, medium strength</t>
+  </si>
+  <si>
+    <t>aluminium production, primary, ingot</t>
+  </si>
+  <si>
+    <t>market for aluminium, primary, ingot</t>
+  </si>
+  <si>
+    <t>sheet rolling, aluminium</t>
+  </si>
+  <si>
+    <t>market for chemical factory, organics</t>
+  </si>
+  <si>
+    <t>chemical factory construction, organics</t>
   </si>
   <si>
     <t>ethylene glycol production</t>
@@ -112,141 +137,210 @@
     <t>polyacrylamide production</t>
   </si>
   <si>
+    <t>market for polyacrylamide</t>
+  </si>
+  <si>
     <t>oxidation of methanol</t>
   </si>
   <si>
     <t>copper sulfate production</t>
   </si>
   <si>
+    <t>market for copper sulfate</t>
+  </si>
+  <si>
     <t>sulfuric acid production</t>
   </si>
   <si>
+    <t>market for sulfuric acid</t>
+  </si>
+  <si>
     <t>dimethylamine production</t>
   </si>
   <si>
+    <t>market for dimethylamine</t>
+  </si>
+  <si>
+    <t>market for ethylene dichloride</t>
+  </si>
+  <si>
     <t>ethylene dichloride production</t>
   </si>
   <si>
     <t>potassium hydroxide production</t>
   </si>
   <si>
+    <t>market for potassium hydroxide</t>
+  </si>
+  <si>
+    <t>market for activated carbon, granular</t>
+  </si>
+  <si>
     <t>activated carbon production, granular from hard coal</t>
   </si>
   <si>
     <t>sodium persulfate production</t>
   </si>
   <si>
-    <t>polydimethylsiloxane production</t>
-  </si>
-  <si>
-    <t>polycarbonate production</t>
+    <t>market for sodium persulfate</t>
+  </si>
+  <si>
+    <t>market for polypropylene, granulate</t>
   </si>
   <si>
     <t>polypropylene production, granulate</t>
   </si>
   <si>
-    <t>polyurethane adhesive production</t>
+    <t>polyvinylchloride production, suspension polymerisation</t>
+  </si>
+  <si>
+    <t>polyvinylchloride production, emulsion polymerisation</t>
+  </si>
+  <si>
+    <t>market for epoxy resin, liquid</t>
+  </si>
+  <si>
+    <t>epoxy resin production, liquid</t>
+  </si>
+  <si>
+    <t>market for polysulfone</t>
+  </si>
+  <si>
+    <t>polysulfone production, for membrane filtration production</t>
+  </si>
+  <si>
+    <t>injection moulding</t>
+  </si>
+  <si>
+    <t>extrusion, plastic pipes</t>
+  </si>
+  <si>
+    <t>extrusion, plastic film</t>
+  </si>
+  <si>
+    <t>textile production, nonwoven polyester, needle-punched</t>
+  </si>
+  <si>
+    <t>market for acrylic varnish, without water, in 87.5% solution state</t>
+  </si>
+  <si>
+    <t>acrylic varnish production, product in 87.5% solution state</t>
+  </si>
+  <si>
+    <t>market for chromium steel pipe</t>
+  </si>
+  <si>
+    <t>market for air compressor, screw-type compressor, 4kW</t>
+  </si>
+  <si>
+    <t>air compressor production, screw-type compressor, 4kW</t>
+  </si>
+  <si>
+    <t>portafer production</t>
+  </si>
+  <si>
+    <t>wood chips production, softwood, at sawmill</t>
+  </si>
+  <si>
+    <t>wood chips production, hardwood, at sawmill</t>
+  </si>
+  <si>
+    <t>market for soda ash, dense</t>
+  </si>
+  <si>
+    <t>soda ash, dense, to generic market for neutralising agent</t>
+  </si>
+  <si>
+    <t>calcium carbonate production, precipitated</t>
+  </si>
+  <si>
+    <t>market for calcium carbonate, precipitated</t>
+  </si>
+  <si>
+    <t>reinforcing steel production</t>
+  </si>
+  <si>
+    <t>market for pump, 40W</t>
+  </si>
+  <si>
+    <t>market for water pump, 22kW</t>
+  </si>
+  <si>
+    <t>market for polyethylene, high density, granulate</t>
   </si>
   <si>
     <t>polyethylene production, high density, granulate</t>
   </si>
   <si>
-    <t>polyethylene production, low density, granulate</t>
-  </si>
-  <si>
-    <t>polyvinylchloride production, suspension polymerisation</t>
-  </si>
-  <si>
-    <t>polyvinylchloride production, emulsion polymerisation</t>
-  </si>
-  <si>
-    <t>epoxy resin production, liquid</t>
-  </si>
-  <si>
-    <t>polysulfone production, for membrane filtration production</t>
-  </si>
-  <si>
-    <t>glass fibre reinforced plastic production, polyester resin, hand lay-up</t>
-  </si>
-  <si>
-    <t>synthetic rubber production</t>
-  </si>
-  <si>
-    <t>tetrafluoroethylene production</t>
-  </si>
-  <si>
-    <t>polyvinylfluoride, film production</t>
-  </si>
-  <si>
-    <t>injection moulding</t>
-  </si>
-  <si>
-    <t>extrusion, plastic pipes</t>
-  </si>
-  <si>
-    <t>storage production, 650 l mini CHP plant</t>
-  </si>
-  <si>
-    <t>textile production, nonwoven polyester, needle-punched</t>
-  </si>
-  <si>
-    <t>acrylic varnish production, product in 87.5% solution state</t>
-  </si>
-  <si>
-    <t>chromium steel pipe production</t>
-  </si>
-  <si>
-    <t>air compressor production, screw-type compressor, 4kW</t>
-  </si>
-  <si>
-    <t>portafer production</t>
-  </si>
-  <si>
-    <t>wood chips production, softwood, at sawmill</t>
-  </si>
-  <si>
-    <t>wood chips production, hardwood, at sawmill</t>
-  </si>
-  <si>
-    <t>soda ash, dense, to generic market for neutralising agent</t>
-  </si>
-  <si>
-    <t>calcium carbonate production, precipitated</t>
-  </si>
-  <si>
-    <t>heat pump production, for mini CHP plant</t>
-  </si>
-  <si>
-    <t>mini CHP plant construction, common components for heat+electricity</t>
-  </si>
-  <si>
-    <t>mini CHP plant production, components for heat only</t>
-  </si>
-  <si>
-    <t>mini CHP plant production, components for electricity only</t>
-  </si>
-  <si>
-    <t>gas boiler production</t>
-  </si>
-  <si>
-    <t>water pump production, 22kW</t>
-  </si>
-  <si>
-    <t>pump production, 40W</t>
-  </si>
-  <si>
-    <t>polyethylene pipe production, corrugated, DN 75</t>
-  </si>
-  <si>
-    <t>polyethylene pipe production, DN 200, SDR 41</t>
+    <t>heat and power co-generation, natural gas, conventional power plant, 100MW electrical</t>
+  </si>
+  <si>
+    <t>heat and power co-generation, oil</t>
+  </si>
+  <si>
+    <t>market for plastic processing factory</t>
   </si>
   <si>
     <t>electricity, high voltage, production mix</t>
   </si>
   <si>
+    <t>market for electricity, low voltage</t>
+  </si>
+  <si>
+    <t>market for electricity, high voltage</t>
+  </si>
+  <si>
+    <t>market for electricity, medium voltage</t>
+  </si>
+  <si>
     <t>heat production, natural gas, at boiler modulating &lt;100kW</t>
   </si>
   <si>
+    <t>heat production, natural gas, at boiler condensing modulating &lt;100kW</t>
+  </si>
+  <si>
+    <t>heat production, natural gas, at boiler atmospheric non-modulating &lt;100kW</t>
+  </si>
+  <si>
+    <t>heat production, natural gas, at boiler fan burner non-modulating &lt;100kW</t>
+  </si>
+  <si>
+    <t>heat production, natural gas, at boiler atmospheric low-NOx non-modulating &lt;100kW</t>
+  </si>
+  <si>
+    <t>heat production, natural gas, at boiler fan burner low-NOx non-modulating &lt;100kW</t>
+  </si>
+  <si>
+    <t>heat production, natural gas, at boiler atm. low-NOx condensing non-modulating &lt;100kW</t>
+  </si>
+  <si>
+    <t>market for transport, freight, lorry 3.5-7.5 metric ton, EURO4</t>
+  </si>
+  <si>
+    <t>market for transport, freight, lorry 3.5-7.5 metric ton, EURO3</t>
+  </si>
+  <si>
+    <t>market for transport, freight, lorry 3.5-7.5 metric ton, EURO5</t>
+  </si>
+  <si>
+    <t>market for transport, freight, lorry 3.5-7.5 metric ton, EURO6</t>
+  </si>
+  <si>
+    <t>transport, freight, lorry 3.5-7.5 metric ton, EURO6</t>
+  </si>
+  <si>
+    <t>transport, freight, lorry 3.5-7.5 metric ton, EURO4</t>
+  </si>
+  <si>
+    <t>transport, freight, lorry 3.5-7.5 metric ton, EURO5</t>
+  </si>
+  <si>
+    <t>transport, freight, lorry 3.5-7.5 metric ton, EURO3</t>
+  </si>
+  <si>
+    <t>market for natural gas, low pressure</t>
+  </si>
+  <si>
     <t>kilogram</t>
   </si>
   <si>
@@ -256,13 +350,13 @@
     <t>unit</t>
   </si>
   <si>
-    <t>meter</t>
+    <t>megajoule</t>
   </si>
   <si>
     <t>kilowatt hour</t>
   </si>
   <si>
-    <t>megajoule</t>
+    <t>ton kilometer</t>
   </si>
   <si>
     <t>kg SO2-Eq</t>
@@ -287,6 +381,117 @@
   </si>
   <si>
     <t>kg O3-Eq</t>
+  </si>
+  <si>
+    <t>stainless_steel</t>
+  </si>
+  <si>
+    <t>rockwool</t>
+  </si>
+  <si>
+    <t>slab_concrete</t>
+  </si>
+  <si>
+    <t>wall_concrete</t>
+  </si>
+  <si>
+    <t>ImpactItem</t>
+  </si>
+  <si>
+    <t>aluminum_sheet</t>
+  </si>
+  <si>
+    <t>chemical_factory</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>MAA</t>
+  </si>
+  <si>
+    <t>PAM</t>
+  </si>
+  <si>
+    <t>FMD</t>
+  </si>
+  <si>
+    <t>CuSO4</t>
+  </si>
+  <si>
+    <t>H2SO4</t>
+  </si>
+  <si>
+    <t>DMA</t>
+  </si>
+  <si>
+    <t>EDCl</t>
+  </si>
+  <si>
+    <t>KOH</t>
+  </si>
+  <si>
+    <t>GAC</t>
+  </si>
+  <si>
+    <t>NaPS</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>PVC</t>
+  </si>
+  <si>
+    <t>epoxy</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>molding</t>
+  </si>
+  <si>
+    <t>extrusion</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>varnish</t>
+  </si>
+  <si>
+    <t>air_compressor</t>
+  </si>
+  <si>
+    <t>iron_sponge</t>
+  </si>
+  <si>
+    <t>carbon_steel</t>
+  </si>
+  <si>
+    <t>pump_40W</t>
+  </si>
+  <si>
+    <t>pump_22kW</t>
+  </si>
+  <si>
+    <t>HDPE_pipes</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>heat</t>
+  </si>
+  <si>
+    <t>heat_onsite</t>
+  </si>
+  <si>
+    <t>trucking</t>
+  </si>
+  <si>
+    <t>biogas_offset</t>
   </si>
 </sst>
 </file>
@@ -318,7 +523,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -341,16 +546,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -691,19 +910,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.62890625" customWidth="1"/>
-    <col min="2" max="2" width="56.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -721,7 +940,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -755,7 +974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
@@ -790,40 +1009,43 @@
       <c r="L3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M3" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="F5" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="H5" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="J5" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="K5" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="L5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -831,37 +1053,40 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D6">
-        <v>2.4085729889497871E-2</v>
+        <v>2.4209695330257811E-2</v>
       </c>
       <c r="E6">
-        <v>5.1444365194698207</v>
+        <v>5.1493196529397487</v>
       </c>
       <c r="F6">
-        <v>227.2801733247853</v>
+        <v>227.42745911975641</v>
       </c>
       <c r="G6">
-        <v>1.5590115820941429E-2</v>
+        <v>1.5689202345125591E-2</v>
       </c>
       <c r="H6">
-        <v>1.1285493661662921E-5</v>
+        <v>1.127964377646976E-5</v>
       </c>
       <c r="I6">
-        <v>2.912714304720448E-6</v>
+        <v>2.9172640916559248E-6</v>
       </c>
       <c r="J6">
-        <v>2.358700519480213E-7</v>
+        <v>2.4332095374862222E-7</v>
       </c>
       <c r="K6">
-        <v>1.513020070136867E-2</v>
+        <v>1.5070707936032971E-2</v>
       </c>
       <c r="L6">
-        <v>0.29924253090808589</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.303451916953484</v>
+      </c>
+      <c r="M6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -869,37 +1094,40 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D7">
-        <v>1.5523619695133691E-2</v>
+        <v>2.508518863485373E-2</v>
       </c>
       <c r="E7">
-        <v>4.5125171699470039</v>
+        <v>5.4057546042736853</v>
       </c>
       <c r="F7">
-        <v>17.718876290230021</v>
+        <v>234.0579121859308</v>
       </c>
       <c r="G7">
-        <v>4.3923343228409427E-3</v>
+        <v>1.6492257512791111E-2</v>
       </c>
       <c r="H7">
-        <v>1.6606105948777239E-7</v>
+        <v>1.151169013567885E-5</v>
       </c>
       <c r="I7">
-        <v>3.172111521361451E-7</v>
+        <v>2.9674173787391831E-6</v>
       </c>
       <c r="J7">
-        <v>1.13995168713347E-7</v>
+        <v>2.6269401232071878E-7</v>
       </c>
       <c r="K7">
-        <v>1.8185582574941741E-3</v>
+        <v>1.538950384396132E-2</v>
       </c>
       <c r="L7">
-        <v>0.2046859087406348</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.31844067923542863</v>
+      </c>
+      <c r="M7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -907,37 +1135,40 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D8">
-        <v>8.3554630099028897E-3</v>
+        <v>9.3355095124370534E-3</v>
       </c>
       <c r="E8">
-        <v>1.105064807573692</v>
+        <v>1.3051141722884121</v>
       </c>
       <c r="F8">
-        <v>15.08019696081209</v>
+        <v>16.386162630999898</v>
       </c>
       <c r="G8">
-        <v>2.9990236640309569E-3</v>
+        <v>3.7590468323049119E-3</v>
       </c>
       <c r="H8">
-        <v>7.161726191861093E-8</v>
+        <v>8.1338274780934293E-8</v>
       </c>
       <c r="I8">
-        <v>2.22618878086666E-7</v>
+        <v>2.6797675004417982E-7</v>
       </c>
       <c r="J8">
-        <v>8.0390210940748158E-8</v>
+        <v>8.095898616556542E-8</v>
       </c>
       <c r="K8">
-        <v>1.2146431206648831E-3</v>
+        <v>1.569606825346523E-3</v>
       </c>
       <c r="L8">
-        <v>6.6262377561846802E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>8.1372437681979146E-2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -945,37 +1176,40 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D9">
-        <v>1.6489182981534571E-3</v>
+        <v>9.6116298698812989E-3</v>
       </c>
       <c r="E9">
-        <v>0.26305090157694982</v>
+        <v>1.370759389808792</v>
       </c>
       <c r="F9">
-        <v>8.3810177569100652</v>
+        <v>17.148693210287579</v>
       </c>
       <c r="G9">
-        <v>1.395340465276369E-3</v>
+        <v>3.9299328830739106E-3</v>
       </c>
       <c r="H9">
-        <v>8.4978934966396428E-8</v>
+        <v>8.6393237172769242E-8</v>
       </c>
       <c r="I9">
-        <v>1.4291219446606219E-7</v>
+        <v>2.8233714722544502E-7</v>
       </c>
       <c r="J9">
-        <v>1.9750856610726991E-8</v>
+        <v>8.5592959174193769E-8</v>
       </c>
       <c r="K9">
-        <v>3.5808967848407819E-4</v>
+        <v>1.6240034226810661E-3</v>
       </c>
       <c r="L9">
-        <v>2.2306645702629541E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>8.5368767420522559E-2</v>
+      </c>
+      <c r="M9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -983,7 +1217,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D10">
         <v>3.0811986745389062</v>
@@ -1012,8 +1246,11 @@
       <c r="L10">
         <v>46.742932603631438</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="M10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -1021,37 +1258,40 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D11">
-        <v>0.57516520443394314</v>
+        <v>0.82938046730130888</v>
       </c>
       <c r="E11">
-        <v>220.32266058350879</v>
+        <v>288.40492066261532</v>
       </c>
       <c r="F11">
-        <v>1468.3351291761769</v>
+        <v>1942.08887046629</v>
       </c>
       <c r="G11">
-        <v>0.25952568992956759</v>
+        <v>0.33882363429196</v>
       </c>
       <c r="H11">
-        <v>8.9383360297347111E-6</v>
+        <v>1.195943784985053E-5</v>
       </c>
       <c r="I11">
-        <v>3.4360326719240329E-5</v>
+        <v>4.5919846995345983E-5</v>
       </c>
       <c r="J11">
-        <v>1.2168418911730101E-5</v>
+        <v>1.9960190839033221E-5</v>
       </c>
       <c r="K11">
-        <v>9.0748012672979078E-2</v>
+        <v>0.12301720090215131</v>
       </c>
       <c r="L11">
-        <v>12.00712352370936</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>17.515903237468901</v>
+      </c>
+      <c r="M11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1059,37 +1299,40 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D12">
-        <v>0.58162607988276849</v>
+        <v>1.0163964735698601</v>
       </c>
       <c r="E12">
-        <v>223.28407443230029</v>
+        <v>381.71826042571172</v>
       </c>
       <c r="F12">
-        <v>1469.402806383735</v>
+        <v>2321.5620129348181</v>
       </c>
       <c r="G12">
-        <v>0.26388755130809899</v>
+        <v>0.43633611623678642</v>
       </c>
       <c r="H12">
-        <v>9.0056617384669633E-6</v>
+        <v>1.4028598068183219E-5</v>
       </c>
       <c r="I12">
-        <v>3.4324480238451869E-5</v>
+        <v>5.7409862290089733E-5</v>
       </c>
       <c r="J12">
-        <v>1.2394617895234129E-5</v>
+        <v>2.32729600635565E-5</v>
       </c>
       <c r="K12">
-        <v>9.179022079643985E-2</v>
+        <v>0.15157516107722699</v>
       </c>
       <c r="L12">
-        <v>12.19020931143892</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>21.160787621427001</v>
+      </c>
+      <c r="M12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1097,37 +1340,40 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>102</v>
       </c>
       <c r="D13">
-        <v>0.77039105635651262</v>
+        <v>0.1670092164462503</v>
       </c>
       <c r="E13">
-        <v>322.72299966376431</v>
+        <v>20.609776437249369</v>
       </c>
       <c r="F13">
-        <v>1869.8112042619709</v>
+        <v>322.59862896811501</v>
       </c>
       <c r="G13">
-        <v>0.36270569459337709</v>
+        <v>0.10536777332018719</v>
       </c>
       <c r="H13">
-        <v>1.116314224810161E-5</v>
+        <v>5.9543187237856376E-6</v>
       </c>
       <c r="I13">
-        <v>4.6709474943059757E-5</v>
+        <v>9.0820361937783114E-6</v>
       </c>
       <c r="J13">
-        <v>1.5806902040845719E-5</v>
+        <v>6.3509069903705737E-7</v>
       </c>
       <c r="K13">
-        <v>0.12141386193929379</v>
+        <v>3.0728095767409501E-2</v>
       </c>
       <c r="L13">
-        <v>15.931775197425949</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>1.5067583954021051</v>
+      </c>
+      <c r="M13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -1135,37 +1381,40 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D14">
-        <v>6.0073414373162277E-3</v>
+        <v>0.1233299852782053</v>
       </c>
       <c r="E14">
-        <v>1.8483461560665131</v>
+        <v>21.576173953409018</v>
       </c>
       <c r="F14">
-        <v>27.371609427023628</v>
+        <v>270.6055097191275</v>
       </c>
       <c r="G14">
-        <v>4.8295406775385446E-3</v>
+        <v>5.6465486785752868E-2</v>
       </c>
       <c r="H14">
-        <v>1.273329431053593E-7</v>
+        <v>5.8303052281387794E-6</v>
       </c>
       <c r="I14">
-        <v>3.9163793607762248E-7</v>
+        <v>5.7425425304895304E-6</v>
       </c>
       <c r="J14">
-        <v>3.2738190094168279E-8</v>
+        <v>6.9973810967502863E-7</v>
       </c>
       <c r="K14">
-        <v>7.0254063796938433E-4</v>
+        <v>2.2744287819579101E-2</v>
       </c>
       <c r="L14">
-        <v>7.9512554236612007E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>1.4517405088141899</v>
+      </c>
+      <c r="M14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -1173,37 +1422,40 @@
         <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D15">
-        <v>3.5128570270090559E-2</v>
+        <v>2.8878712518524922E-3</v>
       </c>
       <c r="E15">
-        <v>6.6971545942522166</v>
+        <v>0.66711843338449983</v>
       </c>
       <c r="F15">
-        <v>166.8803038722661</v>
+        <v>9.3825586774623169</v>
       </c>
       <c r="G15">
-        <v>2.108166734939244E-2</v>
+        <v>1.9679005786980008E-3</v>
       </c>
       <c r="H15">
-        <v>4.4273250866850481E-7</v>
+        <v>7.3576994668512034E-8</v>
       </c>
       <c r="I15">
-        <v>2.636101200242338E-6</v>
+        <v>1.453060953739666E-7</v>
       </c>
       <c r="J15">
-        <v>2.6471232081379171E-7</v>
+        <v>3.1250550801076991E-8</v>
       </c>
       <c r="K15">
-        <v>4.8441449558429888E-3</v>
+        <v>8.2093774932036432E-4</v>
       </c>
       <c r="L15">
-        <v>0.33054909538710009</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>3.8548435253125943E-2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -1211,37 +1463,40 @@
         <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="D16">
-        <v>1.4783903305839801E-2</v>
+        <v>1427643.621415674</v>
       </c>
       <c r="E16">
-        <v>3.2191182512047418</v>
+        <v>156578811.48842201</v>
       </c>
       <c r="F16">
-        <v>30.975436109677041</v>
+        <v>26067081460.813751</v>
       </c>
       <c r="G16">
-        <v>1.5949519001672258E-2</v>
+        <v>1218632.638544189</v>
       </c>
       <c r="H16">
-        <v>1.534463659698768E-7</v>
+        <v>84.540025391624425</v>
       </c>
       <c r="I16">
-        <v>5.037846155016643E-7</v>
+        <v>290.88920092825509</v>
       </c>
       <c r="J16">
-        <v>1.142904467987489E-7</v>
+        <v>8.9289543367295536</v>
       </c>
       <c r="K16">
-        <v>1.5962874087129711E-3</v>
+        <v>265378.68784329097</v>
       </c>
       <c r="L16">
-        <v>0.126040478375435</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>11642162.358833199</v>
+      </c>
+      <c r="M16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -1249,37 +1504,40 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="D17">
-        <v>3.3897172809095951E-3</v>
+        <v>1362751.876595981</v>
       </c>
       <c r="E17">
-        <v>0.87011861083147213</v>
+        <v>144304784.80766499</v>
       </c>
       <c r="F17">
-        <v>13.644208952454941</v>
+        <v>26058754013.985699</v>
       </c>
       <c r="G17">
-        <v>4.0327925094671381E-3</v>
+        <v>1197447.146889837</v>
       </c>
       <c r="H17">
-        <v>6.0299852025642145E-8</v>
+        <v>84.321186743281231</v>
       </c>
       <c r="I17">
-        <v>1.853715322424159E-7</v>
+        <v>290.3899113915719</v>
       </c>
       <c r="J17">
-        <v>2.5453935060748422E-7</v>
+        <v>8.7525689494427752</v>
       </c>
       <c r="K17">
-        <v>3.6205549396033511E-4</v>
+        <v>229382.33662874499</v>
       </c>
       <c r="L17">
-        <v>5.0336292947182781E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>10627401.021839179</v>
+      </c>
+      <c r="M17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>13</v>
       </c>
@@ -1287,37 +1545,40 @@
         <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D18">
-        <v>0.19319265301746821</v>
+        <v>8.675075229211196E-3</v>
       </c>
       <c r="E18">
-        <v>3.7913277856679271</v>
+        <v>2.289762187902463</v>
       </c>
       <c r="F18">
-        <v>5067.9142035823943</v>
+        <v>28.431628192457051</v>
       </c>
       <c r="G18">
-        <v>0.14425878843980189</v>
+        <v>5.0150967421848987E-3</v>
       </c>
       <c r="H18">
-        <v>2.000739661340539E-6</v>
+        <v>1.4544940936056641E-7</v>
       </c>
       <c r="I18">
-        <v>5.2238003764700042E-5</v>
+        <v>4.475422451619449E-7</v>
       </c>
       <c r="J18">
-        <v>2.311108842998087E-7</v>
+        <v>3.9017808879124429E-8</v>
       </c>
       <c r="K18">
-        <v>2.0220403326919711E-2</v>
+        <v>1.839178599730835E-3</v>
       </c>
       <c r="L18">
-        <v>0.72499047355210655</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.11711758875496341</v>
+      </c>
+      <c r="M18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -1325,37 +1586,40 @@
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D19">
-        <v>8.2440945087619948E-3</v>
+        <v>3.5128570270090559E-2</v>
       </c>
       <c r="E19">
-        <v>8.1180873696622163E-2</v>
+        <v>6.6971545942522166</v>
       </c>
       <c r="F19">
-        <v>6.1078043915780702</v>
+        <v>166.8803038722661</v>
       </c>
       <c r="G19">
-        <v>4.052641551952609E-4</v>
+        <v>2.108166734939244E-2</v>
       </c>
       <c r="H19">
-        <v>1.9900118791554861E-8</v>
+        <v>4.4273250866850481E-7</v>
       </c>
       <c r="I19">
-        <v>7.0471539411084789E-8</v>
+        <v>2.636101200242338E-6</v>
       </c>
       <c r="J19">
-        <v>7.8786002778743982E-9</v>
+        <v>2.6471232081379171E-7</v>
       </c>
       <c r="K19">
-        <v>5.3306619619169875E-4</v>
+        <v>4.8441449558429888E-3</v>
       </c>
       <c r="L19">
-        <v>5.0788229739628897E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.33054909538710009</v>
+      </c>
+      <c r="M19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1363,37 +1627,40 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D20">
-        <v>7.9323679736229592E-3</v>
+        <v>1.4783903305839801E-2</v>
       </c>
       <c r="E20">
-        <v>2.4738385941837309</v>
+        <v>3.2191182512047418</v>
       </c>
       <c r="F20">
-        <v>23.839381732285322</v>
+        <v>30.975436109677041</v>
       </c>
       <c r="G20">
-        <v>2.0066526614934108E-2</v>
+        <v>1.5949519001672258E-2</v>
       </c>
       <c r="H20">
-        <v>1.1002785083668409E-7</v>
+        <v>1.534463659698768E-7</v>
       </c>
       <c r="I20">
-        <v>3.3524003279968988E-7</v>
+        <v>5.037846155016643E-7</v>
       </c>
       <c r="J20">
-        <v>5.2855592935421639E-7</v>
+        <v>1.142904467987489E-7</v>
       </c>
       <c r="K20">
-        <v>7.3908156206257849E-4</v>
+        <v>1.5962874087129711E-3</v>
       </c>
       <c r="L20">
-        <v>8.89356054614171E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.126040478375435</v>
+      </c>
+      <c r="M20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -1401,37 +1668,40 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D21">
-        <v>4.0578937885988051E-3</v>
+        <v>1.521896418197302E-2</v>
       </c>
       <c r="E21">
-        <v>0.99626041462335335</v>
+        <v>3.2692635152035332</v>
       </c>
       <c r="F21">
-        <v>23.932736658197271</v>
+        <v>31.37684009508553</v>
       </c>
       <c r="G21">
-        <v>3.6421324206076132E-3</v>
+        <v>1.6024612036162959E-2</v>
       </c>
       <c r="H21">
-        <v>1.014253130810726E-7</v>
+        <v>1.586150041613047E-7</v>
       </c>
       <c r="I21">
-        <v>4.1676460042949509E-7</v>
+        <v>5.1282008766015726E-7</v>
       </c>
       <c r="J21">
-        <v>4.2710039251832932E-7</v>
+        <v>1.2381466326937691E-7</v>
       </c>
       <c r="K21">
-        <v>5.6686092266700614E-4</v>
+        <v>1.6419413125642289E-3</v>
       </c>
       <c r="L21">
-        <v>4.9805082070493327E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.13635889907385179</v>
+      </c>
+      <c r="M21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>17</v>
       </c>
@@ -1439,37 +1709,40 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D22">
-        <v>1.3237645096850119E-2</v>
+        <v>3.6243368374683951E-3</v>
       </c>
       <c r="E22">
-        <v>2.744984314653903</v>
+        <v>0.92048851801375076</v>
       </c>
       <c r="F22">
-        <v>50.724241846065283</v>
+        <v>13.67229449779825</v>
       </c>
       <c r="G22">
-        <v>8.299040852414204E-3</v>
+        <v>3.9774450266166304E-3</v>
       </c>
       <c r="H22">
-        <v>2.4258105073100372E-7</v>
+        <v>6.1014276072633302E-8</v>
       </c>
       <c r="I22">
-        <v>8.3741838603636462E-7</v>
+        <v>1.876759516273198E-7</v>
       </c>
       <c r="J22">
-        <v>1.6299951058807961E-7</v>
+        <v>2.5510452758619319E-7</v>
       </c>
       <c r="K22">
-        <v>3.3362119524061049E-3</v>
+        <v>5.0057798610174615E-4</v>
       </c>
       <c r="L22">
-        <v>0.1739175395086841</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>5.4201750043800817E-2</v>
+      </c>
+      <c r="M22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>18</v>
       </c>
@@ -1477,37 +1750,40 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D23">
-        <v>5.2143502817840658E-2</v>
+        <v>0.19319265301746821</v>
       </c>
       <c r="E23">
-        <v>8.3093636017746011</v>
+        <v>3.7913277856679271</v>
       </c>
       <c r="F23">
-        <v>37.960671101590172</v>
+        <v>5067.9142035823943</v>
       </c>
       <c r="G23">
-        <v>2.6736671732324181E-2</v>
+        <v>0.14425878843980189</v>
       </c>
       <c r="H23">
-        <v>4.1638050250526378E-7</v>
+        <v>2.000739661340539E-6</v>
       </c>
       <c r="I23">
-        <v>1.3938998615257031E-6</v>
+        <v>5.2238003764700042E-5</v>
       </c>
       <c r="J23">
-        <v>1.4034406376134719E-7</v>
+        <v>2.311108842998087E-7</v>
       </c>
       <c r="K23">
-        <v>7.0857398484638614E-3</v>
+        <v>2.0220403326919711E-2</v>
       </c>
       <c r="L23">
-        <v>0.46916640759150208</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.72499047355210655</v>
+      </c>
+      <c r="M23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>19</v>
       </c>
@@ -1515,37 +1791,40 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D24">
-        <v>1.266994614311171E-2</v>
+        <v>0.1935416620435623</v>
       </c>
       <c r="E24">
-        <v>1.510442676050656</v>
+        <v>3.8463859603645592</v>
       </c>
       <c r="F24">
-        <v>84.039229338602951</v>
+        <v>5066.0516504795432</v>
       </c>
       <c r="G24">
-        <v>9.3237811391145703E-3</v>
+        <v>0.14429515656081721</v>
       </c>
       <c r="H24">
-        <v>2.1999799075220221E-7</v>
+        <v>2.0088622183042249E-6</v>
       </c>
       <c r="I24">
-        <v>1.3780940184872829E-6</v>
+        <v>5.2263451479753083E-5</v>
       </c>
       <c r="J24">
-        <v>3.6433854223773832E-7</v>
+        <v>2.4095734342180028E-7</v>
       </c>
       <c r="K24">
-        <v>2.0927910253944831E-3</v>
+        <v>2.0256816257093201E-2</v>
       </c>
       <c r="L24">
-        <v>9.4568009080592055E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.7357597875479932</v>
+      </c>
+      <c r="M24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>20</v>
       </c>
@@ -1553,37 +1832,40 @@
         <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D25">
-        <v>8.1715656946625664E-2</v>
+        <v>8.3277032728490304E-3</v>
       </c>
       <c r="E25">
-        <v>16.695362370857929</v>
+        <v>9.9178611988927134E-2</v>
       </c>
       <c r="F25">
-        <v>151.5957962968786</v>
+        <v>6.1172434740367763</v>
       </c>
       <c r="G25">
-        <v>4.0575422804887983E-2</v>
+        <v>4.0079706333619939E-4</v>
       </c>
       <c r="H25">
-        <v>9.3018620093473582E-7</v>
+        <v>2.0207946998854359E-8</v>
       </c>
       <c r="I25">
-        <v>3.2334374886886982E-6</v>
+        <v>7.180996369377474E-8</v>
       </c>
       <c r="J25">
-        <v>1.5319873459483789E-3</v>
+        <v>8.1442674416377384E-9</v>
       </c>
       <c r="K25">
-        <v>1.5473796307994579E-2</v>
+        <v>5.8167743882602441E-4</v>
       </c>
       <c r="L25">
-        <v>1.1548549689732339</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>6.4387032496995714E-3</v>
+      </c>
+      <c r="M25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>21</v>
       </c>
@@ -1591,37 +1873,40 @@
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D26">
-        <v>2.4322566518315811E-2</v>
+        <v>7.7610403247725989E-3</v>
       </c>
       <c r="E26">
-        <v>7.7850413028470991</v>
+        <v>0.1688709129062175</v>
       </c>
       <c r="F26">
-        <v>13.85372954206886</v>
+        <v>70.135302222458975</v>
       </c>
       <c r="G26">
-        <v>2.563212433018366E-3</v>
+        <v>2.2359984317725139E-3</v>
       </c>
       <c r="H26">
-        <v>2.4786864428792091E-7</v>
+        <v>5.5208317448971632E-8</v>
       </c>
       <c r="I26">
-        <v>8.8123114737693013E-7</v>
+        <v>1.1263306451138381E-6</v>
       </c>
       <c r="J26">
-        <v>4.4611866637081026E-9</v>
+        <v>1.870500675463139E-8</v>
       </c>
       <c r="K26">
-        <v>3.8901585962261868E-3</v>
+        <v>6.5604390682197594E-4</v>
       </c>
       <c r="L26">
-        <v>0.31627244612906141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>2.5092523426939781E-2</v>
+      </c>
+      <c r="M26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>22</v>
       </c>
@@ -1629,37 +1914,40 @@
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D27">
-        <v>5.6119645022909004E-3</v>
+        <v>1.0778755327286071E-2</v>
       </c>
       <c r="E27">
-        <v>1.8608448721471169</v>
+        <v>2.9522238513232919</v>
       </c>
       <c r="F27">
-        <v>15.158814882341369</v>
+        <v>26.22810686382223</v>
       </c>
       <c r="G27">
-        <v>2.0655542316690501E-3</v>
+        <v>2.165781157654767E-2</v>
       </c>
       <c r="H27">
-        <v>8.637056513253151E-8</v>
+        <v>1.3925714072025601E-7</v>
       </c>
       <c r="I27">
-        <v>1.9403017246688381E-7</v>
+        <v>4.4800953131293912E-7</v>
       </c>
       <c r="J27">
-        <v>2.7684150246652811E-8</v>
+        <v>4.3333114842521738E-7</v>
       </c>
       <c r="K27">
-        <v>5.5145870278407844E-4</v>
+        <v>1.5261962928416451E-3</v>
       </c>
       <c r="L27">
-        <v>8.1045763728104875E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.122947919810585</v>
+      </c>
+      <c r="M27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>23</v>
       </c>
@@ -1667,37 +1955,40 @@
         <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D28">
-        <v>2.558611373784361E-2</v>
+        <v>1.121561618073757E-2</v>
       </c>
       <c r="E28">
-        <v>5.4581544258534311</v>
+        <v>3.0025315372327088</v>
       </c>
       <c r="F28">
-        <v>94.876866999385271</v>
+        <v>26.629170500705921</v>
       </c>
       <c r="G28">
-        <v>2.175820274561405E-2</v>
+        <v>2.1732321939085909E-2</v>
       </c>
       <c r="H28">
-        <v>4.6095709976480201E-7</v>
+        <v>1.4441433573328429E-7</v>
       </c>
       <c r="I28">
-        <v>1.558269857075502E-6</v>
+        <v>4.5702890990877918E-7</v>
       </c>
       <c r="J28">
-        <v>7.2012081535820177E-7</v>
+        <v>4.4280410136608898E-7</v>
       </c>
       <c r="K28">
-        <v>5.0274157646736078E-3</v>
+        <v>1.572298904640262E-3</v>
       </c>
       <c r="L28">
-        <v>0.3884110077629116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1333158929891978</v>
+      </c>
+      <c r="M28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>24</v>
       </c>
@@ -1705,37 +1996,40 @@
         <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D29">
-        <v>5.8424163562585344E-3</v>
+        <v>5.8206521811178906E-3</v>
       </c>
       <c r="E29">
-        <v>1.889197380583169</v>
+        <v>1.326807590309061</v>
       </c>
       <c r="F29">
-        <v>15.738275282157391</v>
+        <v>25.012181205589421</v>
       </c>
       <c r="G29">
-        <v>2.466116899168572E-3</v>
+        <v>3.6587765281183792E-3</v>
       </c>
       <c r="H29">
-        <v>1.126000623516756E-7</v>
+        <v>1.130980386415044E-7</v>
       </c>
       <c r="I29">
-        <v>2.136961262996235E-7</v>
+        <v>3.7698510550520721E-7</v>
       </c>
       <c r="J29">
-        <v>4.486790277554288E-8</v>
+        <v>4.3136437991636299E-7</v>
       </c>
       <c r="K29">
-        <v>5.8080933972364619E-4</v>
+        <v>1.326931751200264E-3</v>
       </c>
       <c r="L29">
-        <v>8.5443423095504858E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>7.729747923737719E-2</v>
+      </c>
+      <c r="M29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>25</v>
       </c>
@@ -1743,37 +2037,40 @@
         <v>43</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D30">
-        <v>1.083467201626463E-4</v>
+        <v>5.7394278568156784E-3</v>
       </c>
       <c r="E30">
-        <v>2.8478625916064409E-2</v>
+        <v>1.313761626927346</v>
       </c>
       <c r="F30">
-        <v>0.23448317519761361</v>
+        <v>24.899531473732779</v>
       </c>
       <c r="G30">
-        <v>5.4890928986476407E-5</v>
+        <v>3.639428308641533E-3</v>
       </c>
       <c r="H30">
-        <v>1.5016679470121821E-9</v>
+        <v>1.11681220152167E-7</v>
       </c>
       <c r="I30">
-        <v>4.1466197573786109E-9</v>
+        <v>3.7438784833851681E-7</v>
       </c>
       <c r="J30">
-        <v>4.7471663537593414E-10</v>
+        <v>4.2894170199164599E-7</v>
       </c>
       <c r="K30">
-        <v>1.8890196040183121E-5</v>
+        <v>1.316130304528049E-3</v>
       </c>
       <c r="L30">
-        <v>1.541244719329245E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>7.5153133536033742E-2</v>
+      </c>
+      <c r="M30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>26</v>
       </c>
@@ -1781,37 +2078,40 @@
         <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D31">
-        <v>9.7053818683995909E-3</v>
+        <v>1.3237645096850119E-2</v>
       </c>
       <c r="E31">
-        <v>2.431339071421633</v>
+        <v>2.744984314653903</v>
       </c>
       <c r="F31">
-        <v>40.062615499605947</v>
+        <v>50.724241846065283</v>
       </c>
       <c r="G31">
-        <v>6.0971005043306218E-3</v>
+        <v>8.299040852414204E-3</v>
       </c>
       <c r="H31">
-        <v>1.9166753297345329E-7</v>
+        <v>2.4258105073100372E-7</v>
       </c>
       <c r="I31">
-        <v>6.3272577462748359E-7</v>
+        <v>8.3741838603636462E-7</v>
       </c>
       <c r="J31">
-        <v>1.147692823803628E-6</v>
+        <v>1.6299951058807961E-7</v>
       </c>
       <c r="K31">
-        <v>2.055931900685207E-3</v>
+        <v>3.3362119524061049E-3</v>
       </c>
       <c r="L31">
-        <v>0.12404222539191551</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1739175395086841</v>
+      </c>
+      <c r="M31" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>27</v>
       </c>
@@ -1819,37 +2119,40 @@
         <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D32">
-        <v>8.8439159992618702E-3</v>
+        <v>1.310429589734882E-2</v>
       </c>
       <c r="E32">
-        <v>2.3823753515516799</v>
+        <v>2.7108452112372121</v>
       </c>
       <c r="F32">
-        <v>41.107957525360163</v>
+        <v>50.257008026390551</v>
       </c>
       <c r="G32">
-        <v>6.7225092925464842E-3</v>
+        <v>8.4463805146574623E-3</v>
       </c>
       <c r="H32">
-        <v>1.921305755740457E-7</v>
+        <v>2.4446444493960632E-7</v>
       </c>
       <c r="I32">
-        <v>6.5942261290274099E-7</v>
+        <v>8.2902744106750857E-7</v>
       </c>
       <c r="J32">
-        <v>1.216669575354727E-6</v>
+        <v>1.888263267031637E-7</v>
       </c>
       <c r="K32">
-        <v>1.075782224101125E-3</v>
+        <v>3.0465237783200922E-3</v>
       </c>
       <c r="L32">
-        <v>0.102909495941138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.177057560966557</v>
+      </c>
+      <c r="M32" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>28</v>
       </c>
@@ -1857,37 +2160,40 @@
         <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D33">
-        <v>1.8334257094870209E-2</v>
+        <v>1.9772341446827421E-2</v>
       </c>
       <c r="E33">
-        <v>4.7329324315627961</v>
+        <v>3.284381291709233</v>
       </c>
       <c r="F33">
-        <v>72.750752456212268</v>
+        <v>16.900221487425341</v>
       </c>
       <c r="G33">
-        <v>2.1695862334887552E-2</v>
+        <v>1.0816679996048279E-2</v>
       </c>
       <c r="H33">
-        <v>3.2679188577043363E-7</v>
+        <v>1.67225920078561E-7</v>
       </c>
       <c r="I33">
-        <v>1.0589492607565189E-6</v>
+        <v>6.5822971140763111E-7</v>
       </c>
       <c r="J33">
-        <v>7.4315239446369308E-7</v>
+        <v>1.040905082850221E-7</v>
       </c>
       <c r="K33">
-        <v>3.6123374860579801E-3</v>
+        <v>2.5348041596612971E-3</v>
       </c>
       <c r="L33">
-        <v>0.25703833481078792</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.195327936791162</v>
+      </c>
+      <c r="M33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>29</v>
       </c>
@@ -1895,37 +2201,40 @@
         <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D34">
-        <v>3.0570032379960019E-2</v>
+        <v>5.2143502817840658E-2</v>
       </c>
       <c r="E34">
-        <v>7.5374231306390671</v>
+        <v>8.3093636017746011</v>
       </c>
       <c r="F34">
-        <v>96.108304693822504</v>
+        <v>37.960671101590172</v>
       </c>
       <c r="G34">
-        <v>2.6274536544906021E-2</v>
+        <v>2.6736671732324181E-2</v>
       </c>
       <c r="H34">
-        <v>4.839049346533876E-7</v>
+        <v>4.1638050250526378E-7</v>
       </c>
       <c r="I34">
-        <v>1.5985549319753899E-6</v>
+        <v>1.3938998615257031E-6</v>
       </c>
       <c r="J34">
-        <v>1.102939829597071E-6</v>
+        <v>1.4034406376134719E-7</v>
       </c>
       <c r="K34">
-        <v>6.4903939922454357E-3</v>
+        <v>7.0857398484638614E-3</v>
       </c>
       <c r="L34">
-        <v>0.46080365641305038</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.46916640759150208</v>
+      </c>
+      <c r="M34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>30</v>
       </c>
@@ -1933,37 +2242,40 @@
         <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D35">
-        <v>1.837773173045688E-2</v>
+        <v>1.266994614311171E-2</v>
       </c>
       <c r="E35">
-        <v>4.0364792052818812</v>
+        <v>1.510442676050656</v>
       </c>
       <c r="F35">
-        <v>49.085369762022673</v>
+        <v>84.039229338602951</v>
       </c>
       <c r="G35">
-        <v>1.0770280576346609E-2</v>
+        <v>9.3237811391145703E-3</v>
       </c>
       <c r="H35">
-        <v>2.345644405686527E-7</v>
+        <v>2.1999799075220221E-7</v>
       </c>
       <c r="I35">
-        <v>1.2867664815977479E-6</v>
+        <v>1.3780940184872829E-6</v>
       </c>
       <c r="J35">
-        <v>3.7988190422336329E-7</v>
+        <v>3.6433854223773832E-7</v>
       </c>
       <c r="K35">
-        <v>2.862396526969551E-3</v>
+        <v>2.0927910253944831E-3</v>
       </c>
       <c r="L35">
-        <v>0.26141646303301358</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>9.4568009080592055E-2</v>
+      </c>
+      <c r="M35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>31</v>
       </c>
@@ -1971,37 +2283,40 @@
         <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D36">
-        <v>1.3142923154722579E-2</v>
+        <v>1.310500711394603E-2</v>
       </c>
       <c r="E36">
-        <v>2.80544634987444</v>
+        <v>1.560587950266844</v>
       </c>
       <c r="F36">
-        <v>40.572079413438388</v>
+        <v>84.44063385829665</v>
       </c>
       <c r="G36">
-        <v>7.1859575439039963E-3</v>
+        <v>9.3988742287740082E-3</v>
       </c>
       <c r="H36">
-        <v>2.1203717220722589E-7</v>
+        <v>2.251666210025006E-7</v>
       </c>
       <c r="I36">
-        <v>8.0192505852314772E-7</v>
+        <v>1.3871294988058359E-6</v>
       </c>
       <c r="J36">
-        <v>6.7813608167965557E-7</v>
+        <v>3.7386276074167909E-7</v>
       </c>
       <c r="K36">
-        <v>2.752549812912682E-3</v>
+        <v>2.13844491176108E-3</v>
       </c>
       <c r="L36">
-        <v>0.17076156472354739</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.10488643249509751</v>
+      </c>
+      <c r="M36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>32</v>
       </c>
@@ -2009,37 +2324,40 @@
         <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D37">
-        <v>7.8971147091447518E-4</v>
+        <v>8.2474869389780534E-3</v>
       </c>
       <c r="E37">
-        <v>1.497583267103773</v>
+        <v>2.2345686019567381</v>
       </c>
       <c r="F37">
-        <v>3.991114980327958</v>
+        <v>18.30665843016348</v>
       </c>
       <c r="G37">
-        <v>3.328639574364561E-4</v>
+        <v>3.3907096563938139E-3</v>
       </c>
       <c r="H37">
-        <v>1.063672413906079E-8</v>
+        <v>1.191946735780623E-7</v>
       </c>
       <c r="I37">
-        <v>6.7022443812690574E-8</v>
+        <v>2.9120514163880538E-7</v>
       </c>
       <c r="J37">
-        <v>4.4377564108912738E-5</v>
+        <v>4.7177671863427162E-8</v>
       </c>
       <c r="K37">
-        <v>1.1117054057199091E-4</v>
+        <v>9.9657434587186746E-4</v>
       </c>
       <c r="L37">
-        <v>5.3747762890801482E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1182400840285425</v>
+      </c>
+      <c r="M37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>33</v>
       </c>
@@ -2047,37 +2365,40 @@
         <v>51</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D38">
-        <v>6.9760670440629752E-2</v>
+        <v>5.6119645022909004E-3</v>
       </c>
       <c r="E38">
-        <v>16.435932633480331</v>
+        <v>1.8608448721471169</v>
       </c>
       <c r="F38">
-        <v>230.00896067579939</v>
+        <v>15.158814882341369</v>
       </c>
       <c r="G38">
-        <v>5.2195174187899623E-2</v>
+        <v>2.0655542316690501E-3</v>
       </c>
       <c r="H38">
-        <v>9.3228819424309317E-7</v>
+        <v>8.637056513253151E-8</v>
       </c>
       <c r="I38">
-        <v>4.3051743304767073E-6</v>
+        <v>1.9403017246688381E-7</v>
       </c>
       <c r="J38">
-        <v>1.128703274363726E-6</v>
+        <v>2.7684150246652811E-8</v>
       </c>
       <c r="K38">
-        <v>1.586607216996231E-2</v>
+        <v>5.5145870278407844E-4</v>
       </c>
       <c r="L38">
-        <v>0.93542558645704776</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>8.1045763728104875E-2</v>
+      </c>
+      <c r="M38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>34</v>
       </c>
@@ -2085,37 +2406,40 @@
         <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D39">
-        <v>1.729369817341835E-3</v>
+        <v>9.7053818683995909E-3</v>
       </c>
       <c r="E39">
-        <v>0.53365016395323761</v>
+        <v>2.431339071421633</v>
       </c>
       <c r="F39">
-        <v>4.757248862071684</v>
+        <v>40.062615499605947</v>
       </c>
       <c r="G39">
-        <v>7.1008347110269529E-4</v>
+        <v>6.0971005043306218E-3</v>
       </c>
       <c r="H39">
-        <v>2.9347377458012161E-8</v>
+        <v>1.9166753297345329E-7</v>
       </c>
       <c r="I39">
-        <v>5.2851030390616487E-8</v>
+        <v>6.3272577462748359E-7</v>
       </c>
       <c r="J39">
-        <v>1.8579593526604281E-7</v>
+        <v>1.147692823803628E-6</v>
       </c>
       <c r="K39">
-        <v>1.928125833579233E-4</v>
+        <v>2.055931900685207E-3</v>
       </c>
       <c r="L39">
-        <v>2.2266509013954178E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.12404222539191551</v>
+      </c>
+      <c r="M39" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>35</v>
       </c>
@@ -2123,37 +2447,40 @@
         <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D40">
-        <v>5.8680602720372207E-4</v>
+        <v>1.2207581319197421E-2</v>
       </c>
       <c r="E40">
-        <v>0.12666928515636719</v>
+        <v>2.9867434448251342</v>
       </c>
       <c r="F40">
-        <v>1.7567298611708679</v>
+        <v>43.78226819596037</v>
       </c>
       <c r="G40">
-        <v>2.9222833144640072E-4</v>
+        <v>7.0516525930013714E-3</v>
       </c>
       <c r="H40">
-        <v>2.0666535932371688E-8</v>
+        <v>2.1189309801793999E-7</v>
       </c>
       <c r="I40">
-        <v>2.3443697641855949E-8</v>
+        <v>7.0540134456287082E-7</v>
       </c>
       <c r="J40">
-        <v>1.8086093102872211E-8</v>
+        <v>1.1890089445524639E-6</v>
       </c>
       <c r="K40">
-        <v>8.5712235957590674E-5</v>
+        <v>2.4781622384633692E-3</v>
       </c>
       <c r="L40">
-        <v>6.1015907366098014E-3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1494855228169682</v>
+      </c>
+      <c r="M40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>36</v>
       </c>
@@ -2161,37 +2488,40 @@
         <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="D41">
-        <v>8.083326645578838</v>
+        <v>1.9601917554173429E-2</v>
       </c>
       <c r="E41">
-        <v>1838.642112699057</v>
+        <v>4.9334901248392322</v>
       </c>
       <c r="F41">
-        <v>41884.928290196724</v>
+        <v>73.519545802974307</v>
       </c>
       <c r="G41">
-        <v>5.628505070280263</v>
+        <v>2.162909183849689E-2</v>
       </c>
       <c r="H41">
-        <v>9.7193983960504446E-4</v>
+        <v>3.3556961220739618E-7</v>
       </c>
       <c r="I41">
-        <v>5.8323689390971437E-4</v>
+        <v>1.0837827260925491E-6</v>
       </c>
       <c r="J41">
-        <v>1.5740203519961561E-4</v>
+        <v>7.5231719300365112E-7</v>
       </c>
       <c r="K41">
-        <v>2.0552221910994501</v>
+        <v>4.0807987113399878E-3</v>
       </c>
       <c r="L41">
-        <v>128.10324107041629</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.28182026819226902</v>
+      </c>
+      <c r="M41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>37</v>
       </c>
@@ -2199,37 +2529,40 @@
         <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D42">
-        <v>2.4834726156618161E-2</v>
+        <v>1.9044730646038791E-2</v>
       </c>
       <c r="E42">
-        <v>5.7714418558232783</v>
+        <v>4.853333319968578</v>
       </c>
       <c r="F42">
-        <v>73.445618295573496</v>
+        <v>72.879597715164977</v>
       </c>
       <c r="G42">
-        <v>1.7387778736338899E-2</v>
+        <v>2.152056305053034E-2</v>
       </c>
       <c r="H42">
-        <v>5.5485058431763002E-7</v>
+        <v>3.2883575708844902E-7</v>
       </c>
       <c r="I42">
-        <v>1.4009221001058801E-6</v>
+        <v>1.0677002686469039E-6</v>
       </c>
       <c r="J42">
-        <v>1.442540878762118E-5</v>
+        <v>7.3616782112989461E-7</v>
       </c>
       <c r="K42">
-        <v>5.3729499992496103E-3</v>
+        <v>4.0152271287501179E-3</v>
       </c>
       <c r="L42">
-        <v>0.34757670108633071</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.26831307114652742</v>
+      </c>
+      <c r="M42" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>38</v>
       </c>
@@ -2237,37 +2570,40 @@
         <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D43">
-        <v>1.566139108987959E-2</v>
+        <v>3.100509335716068E-2</v>
       </c>
       <c r="E43">
-        <v>2.6479601501207548</v>
+        <v>7.5875684063117994</v>
       </c>
       <c r="F43">
-        <v>61.146755636986597</v>
+        <v>96.509709120150092</v>
       </c>
       <c r="G43">
-        <v>1.073785332224979E-2</v>
+        <v>2.6349629632715539E-2</v>
       </c>
       <c r="H43">
-        <v>2.1889577708851271E-7</v>
+        <v>4.8907356521517807E-7</v>
       </c>
       <c r="I43">
-        <v>1.0320849524209799E-6</v>
+        <v>1.607590411345561E-6</v>
       </c>
       <c r="J43">
-        <v>2.2953511000388489E-7</v>
+        <v>1.1124640481424631E-6</v>
       </c>
       <c r="K43">
-        <v>2.6667321271850951E-3</v>
+        <v>6.5360478856607354E-3</v>
       </c>
       <c r="L43">
-        <v>0.16779416204456049</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.47112208000392658</v>
+      </c>
+      <c r="M43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>39</v>
       </c>
@@ -2275,37 +2611,40 @@
         <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D44">
-        <v>2.529411095024988E-2</v>
+        <v>3.0570032379960019E-2</v>
       </c>
       <c r="E44">
-        <v>5.5587649312100664</v>
+        <v>7.5374231306390671</v>
       </c>
       <c r="F44">
-        <v>238.51603904599591</v>
+        <v>96.108304693822504</v>
       </c>
       <c r="G44">
-        <v>1.7487302221629201E-2</v>
+        <v>2.6274536544906021E-2</v>
       </c>
       <c r="H44">
-        <v>1.1734112409297401E-5</v>
+        <v>4.839049346533876E-7</v>
       </c>
       <c r="I44">
-        <v>3.0193453571297851E-6</v>
+        <v>1.5985549319753899E-6</v>
       </c>
       <c r="J44">
-        <v>2.6698710974950831E-7</v>
+        <v>1.102939829597071E-6</v>
       </c>
       <c r="K44">
-        <v>1.5390240000981621E-2</v>
+        <v>6.4903939922454357E-3</v>
       </c>
       <c r="L44">
-        <v>0.31847640700611313</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.46080365641305038</v>
+      </c>
+      <c r="M44" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>40</v>
       </c>
@@ -2313,37 +2652,40 @@
         <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="D45">
-        <v>12.073656963151519</v>
+        <v>5.8766195773058433E-3</v>
       </c>
       <c r="E45">
-        <v>793.73422934988741</v>
+        <v>1.4362074990905109</v>
       </c>
       <c r="F45">
-        <v>280525.18743038143</v>
+        <v>10.22654005567577</v>
       </c>
       <c r="G45">
-        <v>9.4116718016510532</v>
+        <v>4.4382247791932977E-3</v>
       </c>
       <c r="H45">
-        <v>7.5720393093265856E-4</v>
+        <v>8.1759094072839719E-8</v>
       </c>
       <c r="I45">
-        <v>2.950386281220684E-3</v>
+        <v>2.5751051551934268E-7</v>
       </c>
       <c r="J45">
-        <v>4.3254825256180202E-5</v>
+        <v>1.110118392144061E-7</v>
       </c>
       <c r="K45">
-        <v>1.8179095397138281</v>
+        <v>1.853397741651893E-3</v>
       </c>
       <c r="L45">
-        <v>73.150321394177197</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>7.769973860128257E-2</v>
+      </c>
+      <c r="M45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>41</v>
       </c>
@@ -2351,37 +2693,43 @@
         <v>59</v>
       </c>
       <c r="C46" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D46">
-        <v>3.1754974359125761E-4</v>
+        <v>2.3462831742591611E-3</v>
       </c>
       <c r="E46">
-        <v>4.3620545619324887E-2</v>
+        <v>0.51797333020845049</v>
       </c>
       <c r="F46">
-        <v>0.31566699560240857</v>
+        <v>3.7881660648094861</v>
       </c>
       <c r="G46">
-        <v>1.2583657005000161E-4</v>
+        <v>1.6990909232195771E-3</v>
       </c>
       <c r="H46">
-        <v>3.207018796531503E-9</v>
+        <v>4.0633047750138382E-8</v>
       </c>
       <c r="I46">
-        <v>8.3999242657780522E-9</v>
+        <v>1.035517746475259E-7</v>
       </c>
       <c r="J46">
-        <v>1.865020805512048E-9</v>
+        <v>1.8747485753837401E-8</v>
       </c>
       <c r="K46">
-        <v>5.0141379990399041E-4</v>
+        <v>6.9816337757760256E-4</v>
       </c>
       <c r="L46">
-        <v>5.5270447981638554E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>2.9051383289355089E-2</v>
+      </c>
+      <c r="M46" t="s">
+        <v>139</v>
+      </c>
+      <c r="N46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>42</v>
       </c>
@@ -2389,37 +2737,40 @@
         <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D47">
-        <v>1.003448479427718E-4</v>
+        <v>2.688267203999708E-3</v>
       </c>
       <c r="E47">
-        <v>2.4105560931567759E-2</v>
+        <v>0.64723677897337217</v>
       </c>
       <c r="F47">
-        <v>0.24121976265892339</v>
+        <v>5.5172956964238198</v>
       </c>
       <c r="G47">
-        <v>1.2961401740341349E-4</v>
+        <v>2.925419839026598E-3</v>
       </c>
       <c r="H47">
-        <v>2.9856582093386632E-9</v>
+        <v>4.2648309451572602E-8</v>
       </c>
       <c r="I47">
-        <v>5.0469385244302284E-9</v>
+        <v>1.4053484823488889E-7</v>
       </c>
       <c r="J47">
-        <v>3.0811543996603108E-9</v>
+        <v>2.4806730531204211E-8</v>
       </c>
       <c r="K47">
-        <v>1.420256057079002E-5</v>
+        <v>8.6980532978985989E-4</v>
       </c>
       <c r="L47">
-        <v>2.3539215776325309E-3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>3.5496128163309923E-2</v>
+      </c>
+      <c r="M47" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43</v>
       </c>
@@ -2427,37 +2778,40 @@
         <v>61</v>
       </c>
       <c r="C48" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D48">
-        <v>1.3586363718418691E-4</v>
+        <v>2.4834726156618161E-2</v>
       </c>
       <c r="E48">
-        <v>2.879392197377053E-2</v>
+        <v>5.7714418558232783</v>
       </c>
       <c r="F48">
-        <v>0.22485623704282001</v>
+        <v>73.445618295573496</v>
       </c>
       <c r="G48">
-        <v>9.7273639058382955E-5</v>
+        <v>1.7387778736338899E-2</v>
       </c>
       <c r="H48">
-        <v>3.2699375172001021E-9</v>
+        <v>5.5485058431763002E-7</v>
       </c>
       <c r="I48">
-        <v>4.9598226163940397E-9</v>
+        <v>1.4009221001058801E-6</v>
       </c>
       <c r="J48">
-        <v>2.3202315639227799E-9</v>
+        <v>1.442540878762118E-5</v>
       </c>
       <c r="K48">
-        <v>3.6893188619067367E-5</v>
+        <v>5.3729499992496103E-3</v>
       </c>
       <c r="L48">
-        <v>2.7123630613338501E-3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.34757670108633071</v>
+      </c>
+      <c r="M48" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44</v>
       </c>
@@ -2465,37 +2819,40 @@
         <v>62</v>
       </c>
       <c r="C49" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D49">
-        <v>6.8910040030967512E-3</v>
+        <v>1.617726031270621E-2</v>
       </c>
       <c r="E49">
-        <v>1.6532762811102719</v>
+        <v>2.7385887276789171</v>
       </c>
       <c r="F49">
-        <v>31.22873764683921</v>
+        <v>62.188207831399517</v>
       </c>
       <c r="G49">
-        <v>8.0388308997974764E-3</v>
+        <v>1.0861454907491779E-2</v>
       </c>
       <c r="H49">
-        <v>1.377273739732079E-7</v>
+        <v>2.2588683199482329E-7</v>
       </c>
       <c r="I49">
-        <v>4.6651458217602198E-7</v>
+        <v>1.054900687956763E-6</v>
       </c>
       <c r="J49">
-        <v>9.4135315104092812E-8</v>
+        <v>2.4858565251623972E-7</v>
       </c>
       <c r="K49">
-        <v>1.264085648386495E-3</v>
+        <v>2.7351943496433479E-3</v>
       </c>
       <c r="L49">
-        <v>0.1038172920574095</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.180239316057307</v>
+      </c>
+      <c r="M49" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45</v>
       </c>
@@ -2503,37 +2860,40 @@
         <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="D50">
-        <v>1.7978724938024109E-3</v>
+        <v>1.566139108987959E-2</v>
       </c>
       <c r="E50">
-        <v>0.33787630406826968</v>
+        <v>2.6479601501207548</v>
       </c>
       <c r="F50">
-        <v>11.135209167145719</v>
+        <v>61.146755636986597</v>
       </c>
       <c r="G50">
-        <v>3.013602884809606E-3</v>
+        <v>1.073785332224979E-2</v>
       </c>
       <c r="H50">
-        <v>3.9777239518568102E-8</v>
+        <v>2.1889577708851271E-7</v>
       </c>
       <c r="I50">
-        <v>1.361537393125253E-7</v>
+        <v>1.0320849524209799E-6</v>
       </c>
       <c r="J50">
-        <v>2.8430519595415051E-8</v>
+        <v>2.2953511000388489E-7</v>
       </c>
       <c r="K50">
-        <v>2.9389134309588911E-4</v>
+        <v>2.6667321271850951E-3</v>
       </c>
       <c r="L50">
-        <v>2.356305240440959E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.16779416204456049</v>
+      </c>
+      <c r="M50" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>46</v>
       </c>
@@ -2541,37 +2901,37 @@
         <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="D51">
-        <v>10.96675446147227</v>
+        <v>2.5590291320571511E-2</v>
       </c>
       <c r="E51">
-        <v>222.03739105475341</v>
+        <v>5.5998208170136916</v>
       </c>
       <c r="F51">
-        <v>288133.39530135121</v>
+        <v>238.84700724637989</v>
       </c>
       <c r="G51">
-        <v>8.3307858410089075</v>
+        <v>1.7545078317147089E-2</v>
       </c>
       <c r="H51">
-        <v>1.9573542077655999E-4</v>
+        <v>1.173793416799605E-5</v>
       </c>
       <c r="I51">
-        <v>3.0168355765251222E-3</v>
+        <v>3.0272741491862731E-6</v>
       </c>
       <c r="J51">
-        <v>1.285933162367626E-5</v>
+        <v>2.7509668862916699E-7</v>
       </c>
       <c r="K51">
-        <v>1.1906933143031191</v>
+        <v>1.542444426626237E-2</v>
       </c>
       <c r="L51">
-        <v>42.417712495063107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.32564188901461749</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>47</v>
       </c>
@@ -2579,37 +2939,40 @@
         <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="D52">
-        <v>17.715975293179049</v>
+        <v>12.074009479215579</v>
       </c>
       <c r="E52">
-        <v>1996.4730784102189</v>
+        <v>786.179227710757</v>
       </c>
       <c r="F52">
-        <v>80529.541872176182</v>
+        <v>280533.62725639768</v>
       </c>
       <c r="G52">
-        <v>5.8868776447763764</v>
+        <v>9.61697260721939</v>
       </c>
       <c r="H52">
-        <v>8.9598754434556905E-4</v>
+        <v>7.5704899111637904E-4</v>
       </c>
       <c r="I52">
-        <v>1.1361135190685141E-3</v>
+        <v>2.9529104327594932E-3</v>
       </c>
       <c r="J52">
-        <v>2.1114453405733191E-4</v>
+        <v>4.3230717954308578E-5</v>
       </c>
       <c r="K52">
-        <v>2.392430623871705</v>
+        <v>1.827449024182042</v>
       </c>
       <c r="L52">
-        <v>154.56538276201681</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>73.157386462631763</v>
+      </c>
+      <c r="M52" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>48</v>
       </c>
@@ -2617,37 +2980,40 @@
         <v>66</v>
       </c>
       <c r="C53" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="D53">
-        <v>41.798208916250637</v>
+        <v>12.074183034055689</v>
       </c>
       <c r="E53">
-        <v>6538.3445226792292</v>
+        <v>782.44809421139553</v>
       </c>
       <c r="F53">
-        <v>473227.82343392831</v>
+        <v>280537.78284646687</v>
       </c>
       <c r="G53">
-        <v>28.527884792017499</v>
+        <v>9.7183616347407309</v>
       </c>
       <c r="H53">
-        <v>2.5388327956498971E-3</v>
+        <v>7.5697243913501889E-4</v>
       </c>
       <c r="I53">
-        <v>5.4850751871178723E-3</v>
+        <v>2.9541568739005798E-3</v>
       </c>
       <c r="J53">
-        <v>4.3768357340257891E-4</v>
+        <v>4.321881044088187E-5</v>
       </c>
       <c r="K53">
-        <v>8.2178165397930432</v>
+        <v>1.8321600935458431</v>
       </c>
       <c r="L53">
-        <v>442.44541478883809</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>73.160872334967877</v>
+      </c>
+      <c r="M53" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>49</v>
       </c>
@@ -2655,37 +3021,40 @@
         <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="D54">
-        <v>7.460321860185827</v>
+        <v>3.1754974359125761E-4</v>
       </c>
       <c r="E54">
-        <v>862.96354071645169</v>
+        <v>4.3620545619324887E-2</v>
       </c>
       <c r="F54">
-        <v>65049.847672636082</v>
+        <v>0.31566699560240857</v>
       </c>
       <c r="G54">
-        <v>3.8834166227687841</v>
+        <v>1.2583657005000161E-4</v>
       </c>
       <c r="H54">
-        <v>2.026175521760005E-4</v>
+        <v>3.207018796531503E-9</v>
       </c>
       <c r="I54">
-        <v>9.0054570177005482E-4</v>
+        <v>8.3999242657780522E-9</v>
       </c>
       <c r="J54">
-        <v>5.9520121118880387E-5</v>
+        <v>1.865020805512048E-9</v>
       </c>
       <c r="K54">
-        <v>1.0734649004664589</v>
+        <v>5.0141379990399041E-4</v>
       </c>
       <c r="L54">
-        <v>65.772156640798912</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>5.5270447981638554E-3</v>
+      </c>
+      <c r="M54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>50</v>
       </c>
@@ -2693,37 +3062,40 @@
         <v>68</v>
       </c>
       <c r="C55" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="D55">
-        <v>4.3408052644170887</v>
+        <v>1.003448479427718E-4</v>
       </c>
       <c r="E55">
-        <v>508.28407955317613</v>
+        <v>2.4105560931567759E-2</v>
       </c>
       <c r="F55">
-        <v>86910.506871515929</v>
+        <v>0.24121976265892339</v>
       </c>
       <c r="G55">
-        <v>3.45761597293273</v>
+        <v>1.2961401740341349E-4</v>
       </c>
       <c r="H55">
-        <v>5.9768738666675641E-4</v>
+        <v>2.9856582093386632E-9</v>
       </c>
       <c r="I55">
-        <v>8.7987270135620236E-4</v>
+        <v>5.0469385244302284E-9</v>
       </c>
       <c r="J55">
-        <v>2.860709891426959E-5</v>
+        <v>3.0811543996603108E-9</v>
       </c>
       <c r="K55">
-        <v>0.89494473894098947</v>
+        <v>1.420256057079002E-5</v>
       </c>
       <c r="L55">
-        <v>36.303510780944848</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>2.3539215776325309E-3</v>
+      </c>
+      <c r="M55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>51</v>
       </c>
@@ -2731,37 +3103,40 @@
         <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="D56">
-        <v>17.938025614823498</v>
+        <v>1.3586363718418691E-4</v>
       </c>
       <c r="E56">
-        <v>1283.1037262435941</v>
+        <v>2.879392197377053E-2</v>
       </c>
       <c r="F56">
-        <v>1573301.7234750569</v>
+        <v>0.22485623704282001</v>
       </c>
       <c r="G56">
-        <v>13.28577068400573</v>
+        <v>9.7273639058382955E-5</v>
       </c>
       <c r="H56">
-        <v>2.4889589639819419E-3</v>
+        <v>3.2699375172001021E-9</v>
       </c>
       <c r="I56">
-        <v>4.4861706195940066E-3</v>
+        <v>4.9598226163940397E-9</v>
       </c>
       <c r="J56">
-        <v>7.5177137059215758E-5</v>
+        <v>2.3202315639227799E-9</v>
       </c>
       <c r="K56">
-        <v>3.7990966488767199</v>
+        <v>3.6893188619067367E-5</v>
       </c>
       <c r="L56">
-        <v>111.08209324813841</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>2.7123630613338501E-3</v>
+      </c>
+      <c r="M56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>52</v>
       </c>
@@ -2769,37 +3144,40 @@
         <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="D57">
-        <v>0.14212227461096291</v>
+        <v>5.200757586534592E-3</v>
       </c>
       <c r="E57">
-        <v>9.2510249269176565</v>
+        <v>1.24775565217249</v>
       </c>
       <c r="F57">
-        <v>3189.5736873935762</v>
+        <v>23.568858093898729</v>
       </c>
       <c r="G57">
-        <v>0.10531292230566761</v>
+        <v>6.0670420368630854E-3</v>
       </c>
       <c r="H57">
-        <v>2.012121634216439E-5</v>
+        <v>1.039451936151731E-7</v>
       </c>
       <c r="I57">
-        <v>3.5992972430286133E-5</v>
+        <v>3.5208646831052352E-7</v>
       </c>
       <c r="J57">
-        <v>5.2616424627118548E-7</v>
+        <v>7.1045518816378095E-8</v>
       </c>
       <c r="K57">
-        <v>2.9716488363209219E-2</v>
+        <v>9.5402688373002803E-4</v>
       </c>
       <c r="L57">
-        <v>0.85457572715826635</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>7.8352671095566831E-2</v>
+      </c>
+      <c r="M57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>53</v>
       </c>
@@ -2807,37 +3185,40 @@
         <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D58">
-        <v>4.2427303129558887E-3</v>
+        <v>6.8910040030967512E-3</v>
       </c>
       <c r="E58">
-        <v>1.045907075826479</v>
+        <v>1.6532762811102719</v>
       </c>
       <c r="F58">
-        <v>20.68704960381945</v>
+        <v>31.22873764683921</v>
       </c>
       <c r="G58">
-        <v>2.6258440202684159E-3</v>
+        <v>8.0388308997974764E-3</v>
       </c>
       <c r="H58">
-        <v>7.9378697614191662E-8</v>
+        <v>1.377273739732079E-7</v>
       </c>
       <c r="I58">
-        <v>2.6982505875321181E-7</v>
+        <v>4.6651458217602198E-7</v>
       </c>
       <c r="J58">
-        <v>3.8003004810527681E-8</v>
+        <v>9.4135315104092812E-8</v>
       </c>
       <c r="K58">
-        <v>5.4855084316208624E-4</v>
+        <v>1.264085648386495E-3</v>
       </c>
       <c r="L58">
-        <v>5.4606298275374193E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>0.1038172920574095</v>
+      </c>
+      <c r="M58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>54</v>
       </c>
@@ -2845,37 +3226,40 @@
         <v>72</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D59">
-        <v>4.2534751237281843E-2</v>
+        <v>1.7978724938024109E-3</v>
       </c>
       <c r="E59">
-        <v>10.036834952923479</v>
+        <v>0.33787630406826968</v>
       </c>
       <c r="F59">
-        <v>185.17769364746439</v>
+        <v>11.135209167145719</v>
       </c>
       <c r="G59">
-        <v>2.8555427451633E-2</v>
+        <v>3.013602884809606E-3</v>
       </c>
       <c r="H59">
-        <v>7.3206176091797782E-7</v>
+        <v>3.9777239518568102E-8</v>
       </c>
       <c r="I59">
-        <v>2.567299609836942E-6</v>
+        <v>1.361537393125253E-7</v>
       </c>
       <c r="J59">
-        <v>3.2246869814908462E-7</v>
+        <v>2.8430519595415051E-8</v>
       </c>
       <c r="K59">
-        <v>6.8671320664443602E-3</v>
+        <v>2.9389134309588911E-4</v>
       </c>
       <c r="L59">
-        <v>0.54896370334877764</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>2.356305240440959E-2</v>
+      </c>
+      <c r="M59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>55</v>
       </c>
@@ -2883,37 +3267,40 @@
         <v>73</v>
       </c>
       <c r="C60" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="D60">
-        <v>2.000310745204657E-3</v>
+        <v>2.2823058414903228E-3</v>
       </c>
       <c r="E60">
-        <v>0.58207696828590905</v>
+        <v>0.39246179841989443</v>
       </c>
       <c r="F60">
-        <v>6.5147445229833831</v>
+        <v>11.977151361489909</v>
       </c>
       <c r="G60">
-        <v>6.1035685990956986E-3</v>
+        <v>3.091105936206475E-3</v>
       </c>
       <c r="H60">
-        <v>6.3544295964226045E-8</v>
+        <v>4.552004649730898E-8</v>
       </c>
       <c r="I60">
-        <v>2.1652695165120729E-7</v>
+        <v>1.592968168043469E-7</v>
       </c>
       <c r="J60">
-        <v>1.8550017361081969E-8</v>
+        <v>3.8632349609101002E-8</v>
       </c>
       <c r="K60">
-        <v>2.5472145819678878E-3</v>
+        <v>3.4626478878744562E-4</v>
       </c>
       <c r="L60">
-        <v>1.8724443118126741E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+        <v>3.4192378982741779E-2</v>
+      </c>
+      <c r="M60" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>56</v>
       </c>
@@ -2921,34 +3308,1150 @@
         <v>74</v>
       </c>
       <c r="C61" t="s">
+        <v>102</v>
+      </c>
+      <c r="D61">
+        <v>7.4616009494021182E-3</v>
+      </c>
+      <c r="E61">
+        <v>2.079392372280477</v>
+      </c>
+      <c r="F61">
+        <v>87.020151385270964</v>
+      </c>
+      <c r="G61">
+        <v>7.7820069101961998E-3</v>
+      </c>
+      <c r="H61">
+        <v>2.5459665737157399E-6</v>
+      </c>
+      <c r="I61">
+        <v>5.8805234371113874E-7</v>
+      </c>
+      <c r="J61">
+        <v>1.2438696420158089E-7</v>
+      </c>
+      <c r="K61">
+        <v>3.2060356226719391E-3</v>
+      </c>
+      <c r="L61">
+        <v>0.13014360089953389</v>
+      </c>
+      <c r="M61" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>57</v>
+      </c>
+      <c r="B62" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" t="s">
+        <v>104</v>
+      </c>
+      <c r="D62">
+        <v>0.14212227461096291</v>
+      </c>
+      <c r="E62">
+        <v>9.2510249269176565</v>
+      </c>
+      <c r="F62">
+        <v>3189.5736873935762</v>
+      </c>
+      <c r="G62">
+        <v>0.10531292230566761</v>
+      </c>
+      <c r="H62">
+        <v>2.012121634216439E-5</v>
+      </c>
+      <c r="I62">
+        <v>3.5992972430286133E-5</v>
+      </c>
+      <c r="J62">
+        <v>5.2616424627118548E-7</v>
+      </c>
+      <c r="K62">
+        <v>2.9716488363209219E-2</v>
+      </c>
+      <c r="L62">
+        <v>0.85457572715826635</v>
+      </c>
+      <c r="M62" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>58</v>
+      </c>
+      <c r="B63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63">
+        <v>17.938025614823498</v>
+      </c>
+      <c r="E63">
+        <v>1283.1037262435941</v>
+      </c>
+      <c r="F63">
+        <v>1573301.7234750569</v>
+      </c>
+      <c r="G63">
+        <v>13.28577068400573</v>
+      </c>
+      <c r="H63">
+        <v>2.4889589639819419E-3</v>
+      </c>
+      <c r="I63">
+        <v>4.4861706195940066E-3</v>
+      </c>
+      <c r="J63">
+        <v>7.5177137059215758E-5</v>
+      </c>
+      <c r="K63">
+        <v>3.7990966488767199</v>
+      </c>
+      <c r="L63">
+        <v>111.08209324813841</v>
+      </c>
+      <c r="M63" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>59</v>
+      </c>
+      <c r="B64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
+        <v>102</v>
+      </c>
+      <c r="D64">
+        <v>8.3779054743482843E-3</v>
+      </c>
+      <c r="E64">
+        <v>2.2669736055854419</v>
+      </c>
+      <c r="F64">
+        <v>18.497923811473559</v>
+      </c>
+      <c r="G64">
+        <v>3.5232805952407371E-3</v>
+      </c>
+      <c r="H64">
+        <v>1.4152138495019781E-7</v>
+      </c>
+      <c r="I64">
+        <v>3.0247797709317258E-7</v>
+      </c>
+      <c r="J64">
+        <v>6.2280352373050547E-8</v>
+      </c>
+      <c r="K64">
+        <v>1.1041359193455661E-3</v>
+      </c>
+      <c r="L64">
+        <v>0.12251667009144809</v>
+      </c>
+      <c r="M64" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>60</v>
+      </c>
+      <c r="B65" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" t="s">
+        <v>102</v>
+      </c>
+      <c r="D65">
+        <v>8.2885774004322794E-3</v>
+      </c>
+      <c r="E65">
+        <v>2.257223050968816</v>
+      </c>
+      <c r="F65">
+        <v>18.357987632825662</v>
+      </c>
+      <c r="G65">
+        <v>3.6380787500227421E-3</v>
+      </c>
+      <c r="H65">
+        <v>1.4001110138392591E-7</v>
+      </c>
+      <c r="I65">
+        <v>3.0352492516850469E-7</v>
+      </c>
+      <c r="J65">
+        <v>4.6291948882622511E-8</v>
+      </c>
+      <c r="K65">
+        <v>1.1470770464636351E-3</v>
+      </c>
+      <c r="L65">
+        <v>0.1145967493049815</v>
+      </c>
+      <c r="M65" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>61</v>
+      </c>
+      <c r="B66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" t="s">
+        <v>105</v>
+      </c>
+      <c r="D66">
+        <v>4.9478420093360831E-5</v>
+      </c>
+      <c r="E66">
+        <v>3.6696960542741602E-2</v>
+      </c>
+      <c r="F66">
+        <v>5.8047195542765953E-2</v>
+      </c>
+      <c r="G66">
+        <v>6.4537275515124831E-6</v>
+      </c>
+      <c r="H66">
+        <v>3.3054134991508768E-10</v>
+      </c>
+      <c r="I66">
+        <v>8.1025136482085165E-10</v>
+      </c>
+      <c r="J66">
+        <v>5.333439665556651E-9</v>
+      </c>
+      <c r="K66">
+        <v>3.468708163703366E-6</v>
+      </c>
+      <c r="L66">
+        <v>8.5144333741911599E-4</v>
+      </c>
+      <c r="M66" t="s">
+        <v>147</v>
+      </c>
+      <c r="N66" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>62</v>
+      </c>
+      <c r="B67" t="s">
         <v>80</v>
       </c>
-      <c r="D61">
-        <v>7.3793076438428723E-5</v>
-      </c>
-      <c r="E61">
-        <v>7.4211120334528327E-2</v>
-      </c>
-      <c r="F61">
-        <v>0.1629409232385339</v>
-      </c>
-      <c r="G61">
-        <v>1.9485050688014222E-5</v>
-      </c>
-      <c r="H61">
-        <v>1.2123422985395279E-9</v>
-      </c>
-      <c r="I61">
-        <v>2.3010230741065661E-9</v>
-      </c>
-      <c r="J61">
-        <v>8.5888518112481996E-9</v>
-      </c>
-      <c r="K61">
-        <v>6.0465437087421874E-6</v>
-      </c>
-      <c r="L61">
-        <v>1.074330522005385E-3</v>
+      <c r="C67" t="s">
+        <v>105</v>
+      </c>
+      <c r="D67">
+        <v>2.1557111259409809E-4</v>
+      </c>
+      <c r="E67">
+        <v>3.629780000978642E-2</v>
+      </c>
+      <c r="F67">
+        <v>8.0022340598958866E-2</v>
+      </c>
+      <c r="G67">
+        <v>2.9407559956761201E-5</v>
+      </c>
+      <c r="H67">
+        <v>5.0923478734806955E-10</v>
+      </c>
+      <c r="I67">
+        <v>1.673514710058869E-9</v>
+      </c>
+      <c r="J67">
+        <v>1.3212134489535319E-8</v>
+      </c>
+      <c r="K67">
+        <v>2.113675578376966E-5</v>
+      </c>
+      <c r="L67">
+        <v>1.20707425973819E-3</v>
+      </c>
+      <c r="M67" t="s">
+        <v>147</v>
+      </c>
+      <c r="N67" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>63</v>
+      </c>
+      <c r="B68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D68">
+        <v>2375694.2456831411</v>
+      </c>
+      <c r="E68">
+        <v>187801286.7374284</v>
+      </c>
+      <c r="F68">
+        <v>44355415286.838531</v>
+      </c>
+      <c r="G68">
+        <v>1683187.943164892</v>
+      </c>
+      <c r="H68">
+        <v>59.040854010160629</v>
+      </c>
+      <c r="I68">
+        <v>475.34942384785762</v>
+      </c>
+      <c r="J68">
+        <v>14.78207330811151</v>
+      </c>
+      <c r="K68">
+        <v>318209.67317122081</v>
+      </c>
+      <c r="L68">
+        <v>17742807.92162098</v>
+      </c>
+      <c r="M68" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>64</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
+        <v>106</v>
+      </c>
+      <c r="D69">
+        <v>8.8291477248829062E-4</v>
+      </c>
+      <c r="E69">
+        <v>0.42357732259870778</v>
+      </c>
+      <c r="F69">
+        <v>3.3866351891349451</v>
+      </c>
+      <c r="G69">
+        <v>3.1323305030769009E-3</v>
+      </c>
+      <c r="H69">
+        <v>3.5039497432100838E-8</v>
+      </c>
+      <c r="I69">
+        <v>1.115426809633034E-7</v>
+      </c>
+      <c r="J69">
+        <v>2.3614714031809311E-8</v>
+      </c>
+      <c r="K69">
+        <v>1.237198686919637E-3</v>
+      </c>
+      <c r="L69">
+        <v>1.3331464919272531E-2</v>
+      </c>
+      <c r="M69" t="s">
+        <v>147</v>
+      </c>
+      <c r="N69" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>65</v>
+      </c>
+      <c r="B70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C70" t="s">
+        <v>106</v>
+      </c>
+      <c r="D70">
+        <v>9.8897652605322E-4</v>
+      </c>
+      <c r="E70">
+        <v>0.42133771686680499</v>
+      </c>
+      <c r="F70">
+        <v>13.60079533747995</v>
+      </c>
+      <c r="G70">
+        <v>3.0951967344671639E-3</v>
+      </c>
+      <c r="H70">
+        <v>3.9408784505528351E-8</v>
+      </c>
+      <c r="I70">
+        <v>1.3688018966819749E-7</v>
+      </c>
+      <c r="J70">
+        <v>2.383246104617156E-8</v>
+      </c>
+      <c r="K70">
+        <v>1.2010466391693311E-3</v>
+      </c>
+      <c r="L70">
+        <v>1.3691226982150541E-2</v>
+      </c>
+      <c r="M70" t="s">
+        <v>147</v>
+      </c>
+      <c r="N70" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>66</v>
+      </c>
+      <c r="B71" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" t="s">
+        <v>106</v>
+      </c>
+      <c r="D71">
+        <v>9.0616865812806317E-4</v>
+      </c>
+      <c r="E71">
+        <v>0.43066170766844231</v>
+      </c>
+      <c r="F71">
+        <v>3.4595938368749009</v>
+      </c>
+      <c r="G71">
+        <v>3.1474093563880869E-3</v>
+      </c>
+      <c r="H71">
+        <v>3.5499388459002188E-8</v>
+      </c>
+      <c r="I71">
+        <v>1.125659957534352E-7</v>
+      </c>
+      <c r="J71">
+        <v>2.4141186071029312E-8</v>
+      </c>
+      <c r="K71">
+        <v>1.241589175868401E-3</v>
+      </c>
+      <c r="L71">
+        <v>1.360234020519039E-2</v>
+      </c>
+      <c r="M71" t="s">
+        <v>147</v>
+      </c>
+      <c r="N71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>67</v>
+      </c>
+      <c r="B72" t="s">
+        <v>85</v>
+      </c>
+      <c r="C72" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72">
+        <v>9.3003300604656649E-4</v>
+      </c>
+      <c r="E72">
+        <v>0.43703211526343022</v>
+      </c>
+      <c r="F72">
+        <v>5.0041120439116806</v>
+      </c>
+      <c r="G72">
+        <v>3.180377599623775E-3</v>
+      </c>
+      <c r="H72">
+        <v>3.6674477238117913E-8</v>
+      </c>
+      <c r="I72">
+        <v>1.18107526294504E-7</v>
+      </c>
+      <c r="J72">
+        <v>2.4327145351589099E-8</v>
+      </c>
+      <c r="K72">
+        <v>1.2512997446476621E-3</v>
+      </c>
+      <c r="L72">
+        <v>1.3766457380699589E-2</v>
+      </c>
+      <c r="M72" t="s">
+        <v>147</v>
+      </c>
+      <c r="N72" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>68</v>
+      </c>
+      <c r="B73" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" t="s">
+        <v>105</v>
+      </c>
+      <c r="D73">
+        <v>6.538978229802514E-5</v>
+      </c>
+      <c r="E73">
+        <v>7.5193650488997552E-2</v>
+      </c>
+      <c r="F73">
+        <v>0.1442360452263208</v>
+      </c>
+      <c r="G73">
+        <v>1.5870410825061641E-5</v>
+      </c>
+      <c r="H73">
+        <v>1.2595672600640501E-9</v>
+      </c>
+      <c r="I73">
+        <v>1.767427064383062E-9</v>
+      </c>
+      <c r="J73">
+        <v>1.250911401190432E-8</v>
+      </c>
+      <c r="K73">
+        <v>7.3566099635920098E-6</v>
+      </c>
+      <c r="L73">
+        <v>1.1858572021680601E-3</v>
+      </c>
+      <c r="M73" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>69</v>
+      </c>
+      <c r="B74" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" t="s">
+        <v>105</v>
+      </c>
+      <c r="D74">
+        <v>7.0597806043721205E-5</v>
+      </c>
+      <c r="E74">
+        <v>7.0877487258844837E-2</v>
+      </c>
+      <c r="F74">
+        <v>0.1528555565800101</v>
+      </c>
+      <c r="G74">
+        <v>1.702980340595029E-5</v>
+      </c>
+      <c r="H74">
+        <v>1.1549945279360709E-9</v>
+      </c>
+      <c r="I74">
+        <v>2.209008199911858E-9</v>
+      </c>
+      <c r="J74">
+        <v>8.1046231338129012E-9</v>
+      </c>
+      <c r="K74">
+        <v>8.1634552838377227E-6</v>
+      </c>
+      <c r="L74">
+        <v>9.7101251782652682E-4</v>
+      </c>
+      <c r="M74" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>70</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
+        <v>105</v>
+      </c>
+      <c r="D75">
+        <v>6.383115106674175E-5</v>
+      </c>
+      <c r="E75">
+        <v>7.5943809887804373E-2</v>
+      </c>
+      <c r="F75">
+        <v>0.13475242490326139</v>
+      </c>
+      <c r="G75">
+        <v>1.3867828687830511E-5</v>
+      </c>
+      <c r="H75">
+        <v>1.2675547993905969E-9</v>
+      </c>
+      <c r="I75">
+        <v>1.652262777583042E-9</v>
+      </c>
+      <c r="J75">
+        <v>1.272741310492902E-8</v>
+      </c>
+      <c r="K75">
+        <v>6.4432268538439797E-6</v>
+      </c>
+      <c r="L75">
+        <v>1.1860423830200981E-3</v>
+      </c>
+      <c r="M75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>71</v>
+      </c>
+      <c r="B76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" t="s">
+        <v>105</v>
+      </c>
+      <c r="D76">
+        <v>6.8502276257432392E-5</v>
+      </c>
+      <c r="E76">
+        <v>7.6639682595999459E-2</v>
+      </c>
+      <c r="F76">
+        <v>0.1470098043362629</v>
+      </c>
+      <c r="G76">
+        <v>1.6292978974026758E-5</v>
+      </c>
+      <c r="H76">
+        <v>1.283789635076439E-9</v>
+      </c>
+      <c r="I76">
+        <v>1.80141593739437E-9</v>
+      </c>
+      <c r="J76">
+        <v>1.27496733541288E-8</v>
+      </c>
+      <c r="K76">
+        <v>7.515412837716417E-6</v>
+      </c>
+      <c r="L76">
+        <v>1.2740821416251701E-3</v>
+      </c>
+      <c r="M76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>72</v>
+      </c>
+      <c r="B77" t="s">
+        <v>90</v>
+      </c>
+      <c r="C77" t="s">
+        <v>105</v>
+      </c>
+      <c r="D77">
+        <v>8.3071377296862174E-5</v>
+      </c>
+      <c r="E77">
+        <v>8.1176915252249432E-2</v>
+      </c>
+      <c r="F77">
+        <v>0.1929743462417022</v>
+      </c>
+      <c r="G77">
+        <v>2.4800680171475081E-5</v>
+      </c>
+      <c r="H77">
+        <v>1.4579086578580421E-9</v>
+      </c>
+      <c r="I77">
+        <v>2.3608619453042982E-9</v>
+      </c>
+      <c r="J77">
+        <v>1.318626913563572E-8</v>
+      </c>
+      <c r="K77">
+        <v>1.1352446224428019E-5</v>
+      </c>
+      <c r="L77">
+        <v>1.5262002795873139E-3</v>
+      </c>
+      <c r="M77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>73</v>
+      </c>
+      <c r="B78" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" t="s">
+        <v>105</v>
+      </c>
+      <c r="D78">
+        <v>9.1203845739551702E-5</v>
+      </c>
+      <c r="E78">
+        <v>8.5069365881744866E-2</v>
+      </c>
+      <c r="F78">
+        <v>0.23893294090878531</v>
+      </c>
+      <c r="G78">
+        <v>3.3027719471892857E-5</v>
+      </c>
+      <c r="H78">
+        <v>1.624468008608522E-9</v>
+      </c>
+      <c r="I78">
+        <v>2.9201099091397648E-9</v>
+      </c>
+      <c r="J78">
+        <v>1.350508769921295E-8</v>
+      </c>
+      <c r="K78">
+        <v>1.5159694386538979E-5</v>
+      </c>
+      <c r="L78">
+        <v>1.5512875432275731E-3</v>
+      </c>
+      <c r="M78" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>74</v>
+      </c>
+      <c r="B79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" t="s">
+        <v>105</v>
+      </c>
+      <c r="D79">
+        <v>7.6162271732268448E-5</v>
+      </c>
+      <c r="E79">
+        <v>7.4474236537941177E-2</v>
+      </c>
+      <c r="F79">
+        <v>0.17704068560052219</v>
+      </c>
+      <c r="G79">
+        <v>2.2783688508000248E-5</v>
+      </c>
+      <c r="H79">
+        <v>1.337530878732343E-9</v>
+      </c>
+      <c r="I79">
+        <v>2.1659283893808208E-9</v>
+      </c>
+      <c r="J79">
+        <v>1.2097494506779511E-8</v>
+      </c>
+      <c r="K79">
+        <v>1.041203271295748E-5</v>
+      </c>
+      <c r="L79">
+        <v>1.4001837114291709E-3</v>
+      </c>
+      <c r="M79" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>75</v>
+      </c>
+      <c r="B80" t="s">
+        <v>93</v>
+      </c>
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80">
+        <v>2.29507148909081E-3</v>
+      </c>
+      <c r="E80">
+        <v>0.53842802853798521</v>
+      </c>
+      <c r="F80">
+        <v>5.37020453325131</v>
+      </c>
+      <c r="G80">
+        <v>6.7217438753165205E-4</v>
+      </c>
+      <c r="H80">
+        <v>4.6687369808393251E-8</v>
+      </c>
+      <c r="I80">
+        <v>1.2937622427314181E-7</v>
+      </c>
+      <c r="J80">
+        <v>1.140611414098456E-7</v>
+      </c>
+      <c r="K80">
+        <v>2.944935776205536E-4</v>
+      </c>
+      <c r="L80">
+        <v>5.2428972384060447E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>76</v>
+      </c>
+      <c r="B81" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D81">
+        <v>3.0734218698908128E-3</v>
+      </c>
+      <c r="E81">
+        <v>0.54420433877152397</v>
+      </c>
+      <c r="F81">
+        <v>5.3821977665002967</v>
+      </c>
+      <c r="G81">
+        <v>7.2923871704241535E-4</v>
+      </c>
+      <c r="H81">
+        <v>4.6919873425095643E-8</v>
+      </c>
+      <c r="I81">
+        <v>1.3080102912909519E-7</v>
+      </c>
+      <c r="J81">
+        <v>1.182734958872205E-7</v>
+      </c>
+      <c r="K81">
+        <v>3.4350296170614401E-4</v>
+      </c>
+      <c r="L81">
+        <v>7.9729151123970485E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>77</v>
+      </c>
+      <c r="B82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" t="s">
+        <v>107</v>
+      </c>
+      <c r="D82">
+        <v>1.885795075730327E-3</v>
+      </c>
+      <c r="E82">
+        <v>0.54157762190596281</v>
+      </c>
+      <c r="F82">
+        <v>5.3758848697732926</v>
+      </c>
+      <c r="G82">
+        <v>6.5097815169954396E-4</v>
+      </c>
+      <c r="H82">
+        <v>4.6762628130176352E-8</v>
+      </c>
+      <c r="I82">
+        <v>1.295067598952604E-7</v>
+      </c>
+      <c r="J82">
+        <v>1.165451573027928E-7</v>
+      </c>
+      <c r="K82">
+        <v>2.9117713157733501E-4</v>
+      </c>
+      <c r="L82">
+        <v>3.7591540785263812E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>78</v>
+      </c>
+      <c r="B83" t="s">
+        <v>96</v>
+      </c>
+      <c r="C83" t="s">
+        <v>107</v>
+      </c>
+      <c r="D83">
+        <v>1.3828914765543899E-3</v>
+      </c>
+      <c r="E83">
+        <v>0.54151781031837443</v>
+      </c>
+      <c r="F83">
+        <v>5.3703254572403134</v>
+      </c>
+      <c r="G83">
+        <v>6.145271175878595E-4</v>
+      </c>
+      <c r="H83">
+        <v>4.6686105903171289E-8</v>
+      </c>
+      <c r="I83">
+        <v>1.2935070370724791E-7</v>
+      </c>
+      <c r="J83">
+        <v>1.140986988694155E-7</v>
+      </c>
+      <c r="K83">
+        <v>2.7801093917642199E-4</v>
+      </c>
+      <c r="L83">
+        <v>2.0091887371789088E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>79</v>
+      </c>
+      <c r="B84" t="s">
+        <v>97</v>
+      </c>
+      <c r="C84" t="s">
+        <v>107</v>
+      </c>
+      <c r="D84">
+        <v>1.3828914765543899E-3</v>
+      </c>
+      <c r="E84">
+        <v>0.54151781031837443</v>
+      </c>
+      <c r="F84">
+        <v>5.3703254572403134</v>
+      </c>
+      <c r="G84">
+        <v>6.145271175878595E-4</v>
+      </c>
+      <c r="H84">
+        <v>4.6686105903171289E-8</v>
+      </c>
+      <c r="I84">
+        <v>1.2935070370724791E-7</v>
+      </c>
+      <c r="J84">
+        <v>1.140986988694155E-7</v>
+      </c>
+      <c r="K84">
+        <v>2.7801093917642199E-4</v>
+      </c>
+      <c r="L84">
+        <v>2.0091887371789088E-2</v>
+      </c>
+      <c r="M84" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>80</v>
+      </c>
+      <c r="B85" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" t="s">
+        <v>107</v>
+      </c>
+      <c r="D85">
+        <v>2.29507148909081E-3</v>
+      </c>
+      <c r="E85">
+        <v>0.53842802853798521</v>
+      </c>
+      <c r="F85">
+        <v>5.37020453325131</v>
+      </c>
+      <c r="G85">
+        <v>6.7217438753165205E-4</v>
+      </c>
+      <c r="H85">
+        <v>4.6687369808393251E-8</v>
+      </c>
+      <c r="I85">
+        <v>1.2937622427314181E-7</v>
+      </c>
+      <c r="J85">
+        <v>1.140611414098456E-7</v>
+      </c>
+      <c r="K85">
+        <v>2.944935776205536E-4</v>
+      </c>
+      <c r="L85">
+        <v>5.2428972384060447E-2</v>
+      </c>
+      <c r="M85" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>81</v>
+      </c>
+      <c r="B86" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" t="s">
+        <v>107</v>
+      </c>
+      <c r="D86">
+        <v>1.885795075730327E-3</v>
+      </c>
+      <c r="E86">
+        <v>0.54157762190596281</v>
+      </c>
+      <c r="F86">
+        <v>5.3758848697732926</v>
+      </c>
+      <c r="G86">
+        <v>6.5097815169954396E-4</v>
+      </c>
+      <c r="H86">
+        <v>4.6762628130176352E-8</v>
+      </c>
+      <c r="I86">
+        <v>1.295067598952604E-7</v>
+      </c>
+      <c r="J86">
+        <v>1.165451573027928E-7</v>
+      </c>
+      <c r="K86">
+        <v>2.9117713157733501E-4</v>
+      </c>
+      <c r="L86">
+        <v>3.7591540785263812E-2</v>
+      </c>
+      <c r="M86" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>82</v>
+      </c>
+      <c r="B87" t="s">
+        <v>100</v>
+      </c>
+      <c r="C87" t="s">
+        <v>107</v>
+      </c>
+      <c r="D87">
+        <v>3.0734218698908128E-3</v>
+      </c>
+      <c r="E87">
+        <v>0.54420433877152397</v>
+      </c>
+      <c r="F87">
+        <v>5.3821977665002967</v>
+      </c>
+      <c r="G87">
+        <v>7.2923871704241535E-4</v>
+      </c>
+      <c r="H87">
+        <v>4.6919873425095643E-8</v>
+      </c>
+      <c r="I87">
+        <v>1.3080102912909519E-7</v>
+      </c>
+      <c r="J87">
+        <v>1.182734958872205E-7</v>
+      </c>
+      <c r="K87">
+        <v>3.4350296170614401E-4</v>
+      </c>
+      <c r="L87">
+        <v>7.9729151123970485E-2</v>
+      </c>
+      <c r="M87" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>83</v>
+      </c>
+      <c r="B88" t="s">
+        <v>101</v>
+      </c>
+      <c r="C88" t="s">
+        <v>103</v>
+      </c>
+      <c r="D88">
+        <v>1.8968986641433371E-3</v>
+      </c>
+      <c r="E88">
+        <v>0.49429163710241453</v>
+      </c>
+      <c r="F88">
+        <v>2.1873279969190809</v>
+      </c>
+      <c r="G88">
+        <v>2.6777672137774021E-4</v>
+      </c>
+      <c r="H88">
+        <v>2.376722084074359E-8</v>
+      </c>
+      <c r="I88">
+        <v>4.2918957297913371E-8</v>
+      </c>
+      <c r="J88">
+        <v>2.9699360068162721E-7</v>
+      </c>
+      <c r="K88">
+        <v>1.539639086009757E-4</v>
+      </c>
+      <c r="L88">
+        <v>2.1564767497220479E-2</v>
+      </c>
+      <c r="M88" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>